<commit_message>
Paper Version 8 Commit
Code to support many changes and updates made in version 8 of the paper. Some of the changes are: adding VLT-Filter (SCT filter profiles with VLT average spectrum for calibration, all 2023 data added, etc.
</commit_message>
<xml_diff>
--- a/Catalog/Catalog-static.xlsx
+++ b/Catalog/Catalog-static.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEE13DB4-1487-4539-BBDF-DE4BC40D6F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780C98ED-F23C-45CB-954E-018CC3A19A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalog-static" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Catalog-static'!$A$1:$O$78</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1255,7 +1258,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1859,9 +1862,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1899,7 +1902,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2005,7 +2008,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2147,18 +2150,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2216,7 +2220,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
@@ -2263,7 +2267,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -2310,7 +2314,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -2357,7 +2361,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -2404,7 +2408,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>42</v>
       </c>
@@ -2451,7 +2455,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
@@ -2498,7 +2502,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -2545,7 +2549,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" s="11" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>58</v>
       </c>
@@ -2592,7 +2596,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>63</v>
       </c>
@@ -2639,7 +2643,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>68</v>
       </c>
@@ -2686,7 +2690,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>74</v>
       </c>
@@ -2733,7 +2737,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>79</v>
       </c>
@@ -2780,7 +2784,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>84</v>
       </c>
@@ -2827,7 +2831,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>89</v>
       </c>
@@ -2874,7 +2878,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>95</v>
       </c>
@@ -2921,7 +2925,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>100</v>
       </c>
@@ -2968,7 +2972,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>105</v>
       </c>
@@ -3015,7 +3019,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -3062,7 +3066,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>115</v>
       </c>
@@ -3109,7 +3113,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>120</v>
       </c>
@@ -3203,7 +3207,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>130</v>
       </c>
@@ -3250,7 +3254,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>136</v>
       </c>
@@ -3297,7 +3301,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>141</v>
       </c>
@@ -3344,7 +3348,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>146</v>
       </c>
@@ -3391,7 +3395,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>152</v>
       </c>
@@ -3438,7 +3442,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>158</v>
       </c>
@@ -3485,7 +3489,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>162</v>
       </c>
@@ -3626,7 +3630,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>176</v>
       </c>
@@ -3673,7 +3677,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>181</v>
       </c>
@@ -3720,7 +3724,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>185</v>
       </c>
@@ -3767,7 +3771,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>190</v>
       </c>
@@ -3814,7 +3818,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>194</v>
       </c>
@@ -3861,7 +3865,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>199</v>
       </c>
@@ -3908,7 +3912,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>204</v>
       </c>
@@ -3955,7 +3959,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>209</v>
       </c>
@@ -4002,7 +4006,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>214</v>
       </c>
@@ -4049,7 +4053,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>219</v>
       </c>
@@ -4096,7 +4100,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>224</v>
       </c>
@@ -4143,7 +4147,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>229</v>
       </c>
@@ -4284,7 +4288,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>244</v>
       </c>
@@ -4331,7 +4335,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
         <v>249</v>
       </c>
@@ -4378,7 +4382,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>254</v>
       </c>
@@ -4425,7 +4429,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>259</v>
       </c>
@@ -4472,7 +4476,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>264</v>
       </c>
@@ -4519,7 +4523,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>269</v>
       </c>
@@ -4566,7 +4570,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>274</v>
       </c>
@@ -4613,7 +4617,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>279</v>
       </c>
@@ -4660,7 +4664,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>284</v>
       </c>
@@ -4707,7 +4711,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>290</v>
       </c>
@@ -4754,7 +4758,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>295</v>
       </c>
@@ -4801,7 +4805,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="57" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>300</v>
       </c>
@@ -4848,7 +4852,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>305</v>
       </c>
@@ -4895,7 +4899,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>310</v>
       </c>
@@ -4942,7 +4946,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>315</v>
       </c>
@@ -4989,7 +4993,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>320</v>
       </c>
@@ -5083,7 +5087,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>330</v>
       </c>
@@ -5130,7 +5134,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>335</v>
       </c>
@@ -5177,7 +5181,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="14" t="s">
         <v>340</v>
       </c>
@@ -5224,7 +5228,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>345</v>
       </c>
@@ -5271,7 +5275,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>350</v>
       </c>
@@ -5318,7 +5322,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="68" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>355</v>
       </c>
@@ -5365,7 +5369,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>360</v>
       </c>
@@ -5412,7 +5416,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="15" t="s">
         <v>365</v>
       </c>
@@ -5459,7 +5463,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>370</v>
       </c>
@@ -5506,7 +5510,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>375</v>
       </c>
@@ -5553,7 +5557,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="73" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="13" t="s">
         <v>380</v>
       </c>
@@ -5600,7 +5604,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="74" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
         <v>385</v>
       </c>
@@ -5647,7 +5651,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>390</v>
       </c>
@@ -5694,7 +5698,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
         <v>395</v>
       </c>
@@ -5741,7 +5745,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
         <v>400</v>
       </c>
@@ -5788,7 +5792,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="78" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
         <v>405</v>
       </c>
@@ -5836,6 +5840,19 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O78" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter val="2023*"/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <customFilters and="1">
+        <customFilter operator="greaterThanOrEqual" val="35"/>
+        <customFilter operator="lessThanOrEqual" val="55"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Research Intermediate Commit - CALIBRATION PROBLEM?
Substantial work done since the ESS paper submission, particularly on profiles and continguous mapping. I also experimented with using only the 632nm channel for continuum on NH3. HOWEVER, SOMEWHERE IN THE PROCESS, THE OVERALL CALIBRATION OF FNH3 HAS SHIFTED AND NOW I GET VALUES ~10-15% HIGHER THAN IN THE PAPER. THIS COMMIT IS TO ENABLE COMPARES THAT MAY REVEAL WHY.
</commit_message>
<xml_diff>
--- a/Catalog/Catalog-static.xlsx
+++ b/Catalog/Catalog-static.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780C98ED-F23C-45CB-954E-018CC3A19A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BF02F5-55D3-4DDE-811F-6F7A0C44EC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,27 @@
     <sheet name="Catalog-static" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Catalog-static'!$A$1:$O$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Catalog-static'!$A$1:$O$100</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="531">
   <si>
     <t>ObsID</t>
   </si>
@@ -1253,6 +1266,369 @@
   </si>
   <si>
     <t>2023-12-17-0240_5-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20231218UTa</t>
+  </si>
+  <si>
+    <t>2023-12-18_00:00:36</t>
+  </si>
+  <si>
+    <t>2023-12-17-2359_9-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0000_6-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0017_8-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20231218UTb</t>
+  </si>
+  <si>
+    <t>2023-12-18_01:22:36</t>
+  </si>
+  <si>
+    <t>2023-12-18-0122_6-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0122_6-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0134_7-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20231218UTc</t>
+  </si>
+  <si>
+    <t>2023-12-18_02:21:24</t>
+  </si>
+  <si>
+    <t>2023-12-18-0221_4-Jupiter_R656G620B632-RGB-Smth-WthBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0221_4-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0235_5-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20231218UTd</t>
+  </si>
+  <si>
+    <t>2023-12-18_03:12:54</t>
+  </si>
+  <si>
+    <t>2023-12-18-0312_8-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0312_9-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0327_6-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20231218UTe</t>
+  </si>
+  <si>
+    <t>2023-12-18_04:16:24</t>
+  </si>
+  <si>
+    <t>2023-12-18-0416_4-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0416_4-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0430_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20231218UTf</t>
+  </si>
+  <si>
+    <t>2023-12-18_05:13:06</t>
+  </si>
+  <si>
+    <t>2023-12-18-0513_1-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0513_1-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-18-0527_0-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20231229UTa</t>
+  </si>
+  <si>
+    <t>2023-12-29_00:48:00</t>
+  </si>
+  <si>
+    <t>'u/10'</t>
+  </si>
+  <si>
+    <t>2023-12-29-0048_0-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-29-0048_0-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-29-0104_2-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20231229UTb</t>
+  </si>
+  <si>
+    <t>2023-12-29_02:07:00</t>
+  </si>
+  <si>
+    <t>2023-12-29-0207_0-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-29-0207_0-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-29-0220_0-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20231229UTc</t>
+  </si>
+  <si>
+    <t>2023-12-29_03:35:48</t>
+  </si>
+  <si>
+    <t>2023-12-29-0335_7-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-29-0335_8-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2023-12-29-0352_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240129UTa</t>
+  </si>
+  <si>
+    <t>2024-01-29_02:07:00</t>
+  </si>
+  <si>
+    <t>2024-01-29-0207_0-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-29-0207_0-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-29-0223_3-Jupiter_R685G550B450-RGB-ClrSmth-WthBal-WV</t>
+  </si>
+  <si>
+    <t>20240129UTb</t>
+  </si>
+  <si>
+    <t>2024-01-29_02:35:36</t>
+  </si>
+  <si>
+    <t>2024-01-29-0235_6-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-29-0235_6-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-29-0248_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240130UTa</t>
+  </si>
+  <si>
+    <t>2024-01-30-0131_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240130UTb</t>
+  </si>
+  <si>
+    <t>20240130UTc</t>
+  </si>
+  <si>
+    <t>2024-01-30_03:22:06</t>
+  </si>
+  <si>
+    <t>2024-01-30-0322_1-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-30-0322_1-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-30-0334_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240131UTa</t>
+  </si>
+  <si>
+    <t>2024-01-31_02:22:30</t>
+  </si>
+  <si>
+    <t>2024-01-31-0222_5-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-31-0222_5-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-31-0236_3-Jupiter_R685G550B450-RGB-ClrSmthWhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240131UTb</t>
+  </si>
+  <si>
+    <t>2024-01-31_02:49:06</t>
+  </si>
+  <si>
+    <t>2024-01-31-0249_1-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-31-0249_1-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-31-0302_3-Jupiter_R685G550B450-RGB-ClrSmthWhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240202UTa</t>
+  </si>
+  <si>
+    <t>2024-02-02_02:17:06</t>
+  </si>
+  <si>
+    <t>2024-02-02-0217_1-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-02-0217_1-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-02-0229_6-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240202UTb</t>
+  </si>
+  <si>
+    <t>2024-02-02_03:19:30</t>
+  </si>
+  <si>
+    <t>2024-02-02-0319_5-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-02-0319_5-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-02-0334_8-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>2024-01-30_01:17:06</t>
+  </si>
+  <si>
+    <t>2024-01-30-0117_1-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-30-0117_1-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-30_02:48:00</t>
+  </si>
+  <si>
+    <t>2024-01-30-0248_0-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-30-0248_0-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-01-30-0306_4-Jupiter_R685G550B450-DR-ST-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240220UTa</t>
+  </si>
+  <si>
+    <t>2024-02-20_01:34:24</t>
+  </si>
+  <si>
+    <t>2024-02-20-0134_3-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-20-0134_4-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-20-0148_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240220UTb</t>
+  </si>
+  <si>
+    <t>2024-02-20_02:00:36</t>
+  </si>
+  <si>
+    <t>2024-02-20-0200_7-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-20-0200_6-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-20-0214_2-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240229UTa</t>
+  </si>
+  <si>
+    <t>2024-02-29_02:03:12</t>
+  </si>
+  <si>
+    <t>2024-02-29-0203_5-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-29-0203_2-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-29-0216_9-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240229UTb</t>
+  </si>
+  <si>
+    <t>2024-02-29_02:29:06</t>
+  </si>
+  <si>
+    <t>2024-02-29-0229_1-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-29-0229_1-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-02-29-0241_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240301UTa</t>
+  </si>
+  <si>
+    <t>2024-03-01_01:54:00</t>
+  </si>
+  <si>
+    <t>2024-03-01-0154_0-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-03-01-0154_0-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-03-01-0207_7-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20240301UTb</t>
+  </si>
+  <si>
+    <t>2024-03-01_02:20:00</t>
+  </si>
+  <si>
+    <t>2024-03-01-0220_0-Jupiter_R656G620B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-03-01-0220_0-Jupiter_R656G647B632-RGB-Smth-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-03-01-0232_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
   </si>
 </sst>
 </file>
@@ -1401,7 +1777,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1623,6 +1999,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1784,7 +2166,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1803,6 +2185,9 @@
     <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2158,17 +2543,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:O78"/>
+  <dimension ref="A1:O102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J80" sqref="J80"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
     <col min="7" max="7" width="8.6328125" customWidth="1"/>
     <col min="8" max="8" width="10.26953125" customWidth="1"/>
   </cols>
@@ -2220,7 +2607,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
@@ -2267,7 +2654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -2314,7 +2701,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -2361,7 +2748,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
@@ -2408,7 +2795,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>42</v>
       </c>
@@ -2455,7 +2842,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>48</v>
       </c>
@@ -2502,54 +2889,54 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>96.8</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>266.3</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>190.1</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L8" s="3">
-        <v>1</v>
-      </c>
-      <c r="M8" s="3" t="s">
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="N8" s="3">
-        <v>1</v>
-      </c>
-      <c r="O8" s="3" t="s">
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="11" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>58</v>
       </c>
@@ -2596,7 +2983,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>63</v>
       </c>
@@ -2643,7 +3030,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>68</v>
       </c>
@@ -2690,7 +3077,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>74</v>
       </c>
@@ -2737,7 +3124,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>79</v>
       </c>
@@ -2784,7 +3171,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>84</v>
       </c>
@@ -2831,54 +3218,54 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15">
         <v>296.2</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15">
         <v>282.5</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15">
         <v>212.7</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="5" t="s">
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" t="s">
         <v>92</v>
       </c>
-      <c r="L15" s="5">
-        <v>1</v>
-      </c>
-      <c r="M15" s="5" t="s">
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15" t="s">
         <v>93</v>
       </c>
-      <c r="N15" s="5">
-        <v>1</v>
-      </c>
-      <c r="O15" s="5" t="s">
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>95</v>
       </c>
@@ -2925,7 +3312,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>100</v>
       </c>
@@ -2972,7 +3359,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>105</v>
       </c>
@@ -3019,144 +3406,144 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="19" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <v>34.9</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>198.9</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="6">
         <v>135.4</v>
       </c>
-      <c r="F19" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="F19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19" t="s">
+      <c r="L19" s="6">
+        <v>1</v>
+      </c>
+      <c r="M19" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19" t="s">
+      <c r="N19" s="6">
+        <v>1</v>
+      </c>
+      <c r="O19" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="17">
         <v>228.2</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="17">
         <v>24.3</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="17">
         <v>321.10000000000002</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="9" t="s">
+      <c r="F20" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="K20" s="9" t="s">
+      <c r="K20" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="L20" s="9">
-        <v>1</v>
-      </c>
-      <c r="M20" s="9" t="s">
+      <c r="L20" s="17">
+        <v>1</v>
+      </c>
+      <c r="M20" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="N20" s="9">
-        <v>1</v>
-      </c>
-      <c r="O20" s="9" t="s">
+      <c r="N20" s="17">
+        <v>1</v>
+      </c>
+      <c r="O20" s="17" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="21" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>0.7</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="6">
         <v>149.4</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="6">
         <v>86.4</v>
       </c>
-      <c r="F21" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="F21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21" t="s">
+      <c r="L21" s="6">
+        <v>1</v>
+      </c>
+      <c r="M21" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="O21" t="s">
+      <c r="N21" s="6">
+        <v>1</v>
+      </c>
+      <c r="O21" s="6" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3207,7 +3594,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>130</v>
       </c>
@@ -3254,7 +3641,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>136</v>
       </c>
@@ -3301,7 +3688,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>141</v>
       </c>
@@ -3348,7 +3735,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>146</v>
       </c>
@@ -3395,7 +3782,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>152</v>
       </c>
@@ -3442,7 +3829,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>158</v>
       </c>
@@ -3489,7 +3876,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>162</v>
       </c>
@@ -3630,7 +4017,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>176</v>
       </c>
@@ -3677,7 +4064,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>181</v>
       </c>
@@ -3724,7 +4111,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>185</v>
       </c>
@@ -3771,7 +4158,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>190</v>
       </c>
@@ -3818,7 +4205,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>194</v>
       </c>
@@ -3865,7 +4252,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>199</v>
       </c>
@@ -3912,7 +4299,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>204</v>
       </c>
@@ -3959,7 +4346,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>209</v>
       </c>
@@ -4006,7 +4393,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>214</v>
       </c>
@@ -4053,7 +4440,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>219</v>
       </c>
@@ -4100,7 +4487,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>224</v>
       </c>
@@ -4147,7 +4534,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="43" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>229</v>
       </c>
@@ -4288,7 +4675,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>244</v>
       </c>
@@ -4335,7 +4722,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="47" spans="1:15" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
         <v>249</v>
       </c>
@@ -4382,7 +4769,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>254</v>
       </c>
@@ -4429,7 +4816,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>259</v>
       </c>
@@ -4476,7 +4863,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>264</v>
       </c>
@@ -4523,7 +4910,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>269</v>
       </c>
@@ -4570,7 +4957,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>274</v>
       </c>
@@ -4617,7 +5004,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>279</v>
       </c>
@@ -4664,7 +5051,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>284</v>
       </c>
@@ -4711,7 +5098,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>290</v>
       </c>
@@ -4758,7 +5145,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>295</v>
       </c>
@@ -4805,7 +5192,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="57" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>300</v>
       </c>
@@ -4852,7 +5239,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>305</v>
       </c>
@@ -4899,7 +5286,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="10" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
         <v>310</v>
       </c>
@@ -4946,7 +5333,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="60" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>315</v>
       </c>
@@ -4993,7 +5380,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>320</v>
       </c>
@@ -5087,7 +5474,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>330</v>
       </c>
@@ -5134,7 +5521,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="64" spans="1:15" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>335</v>
       </c>
@@ -5181,7 +5568,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="14" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="14" t="s">
         <v>340</v>
       </c>
@@ -5228,7 +5615,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>345</v>
       </c>
@@ -5275,7 +5662,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>350</v>
       </c>
@@ -5322,7 +5709,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="68" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>355</v>
       </c>
@@ -5369,7 +5756,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>360</v>
       </c>
@@ -5416,7 +5803,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="15" t="s">
         <v>365</v>
       </c>
@@ -5463,7 +5850,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>370</v>
       </c>
@@ -5510,7 +5897,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>375</v>
       </c>
@@ -5557,7 +5944,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="73" spans="1:15" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="13" t="s">
         <v>380</v>
       </c>
@@ -5604,7 +5991,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="74" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
         <v>385</v>
       </c>
@@ -5651,7 +6038,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>390</v>
       </c>
@@ -5698,7 +6085,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="6" t="s">
         <v>395</v>
       </c>
@@ -5745,7 +6132,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="6" t="s">
         <v>400</v>
       </c>
@@ -5792,7 +6179,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="78" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
         <v>405</v>
       </c>
@@ -5839,20 +6226,1137 @@
         <v>409</v>
       </c>
     </row>
+    <row r="79" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C79" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="D79" s="1">
+        <v>173.1</v>
+      </c>
+      <c r="E79" s="1">
+        <v>222.6</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="L79" s="1">
+        <v>1</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="N79" s="1">
+        <v>1</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C80" s="1">
+        <v>60.6</v>
+      </c>
+      <c r="D80" s="1">
+        <v>222.6</v>
+      </c>
+      <c r="E80" s="1">
+        <v>272.2</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="L80" s="1">
+        <v>1</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="N80" s="1">
+        <v>1</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C81" s="1">
+        <v>96.5</v>
+      </c>
+      <c r="D81" s="1">
+        <v>258.2</v>
+      </c>
+      <c r="E81" s="1">
+        <v>307.7</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="L81" s="1">
+        <v>1</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="N81" s="1">
+        <v>1</v>
+      </c>
+      <c r="O81" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C82" s="1">
+        <v>127.9</v>
+      </c>
+      <c r="D82" s="1">
+        <v>289.3</v>
+      </c>
+      <c r="E82" s="1">
+        <v>338.9</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="L82" s="1">
+        <v>1</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="N82" s="1">
+        <v>1</v>
+      </c>
+      <c r="O82" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C83" s="1">
+        <v>166.6</v>
+      </c>
+      <c r="D83" s="1">
+        <v>327.7</v>
+      </c>
+      <c r="E83" s="1">
+        <v>17.3</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="L83" s="1">
+        <v>1</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="N83" s="1">
+        <v>1</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C84" s="1">
+        <v>201.2</v>
+      </c>
+      <c r="D84" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="E84" s="1">
+        <v>51.5</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="L84" s="1">
+        <v>1</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="N84" s="1">
+        <v>1</v>
+      </c>
+      <c r="O84" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="C85" s="2">
+        <v>335.9</v>
+      </c>
+      <c r="D85" s="2">
+        <v>54.1</v>
+      </c>
+      <c r="E85" s="2">
+        <v>106.6</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="L85" s="2">
+        <v>1</v>
+      </c>
+      <c r="M85" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="N85" s="2">
+        <v>1</v>
+      </c>
+      <c r="O85" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="C86" s="2">
+        <v>24</v>
+      </c>
+      <c r="D86" s="2">
+        <v>101.9</v>
+      </c>
+      <c r="E86" s="2">
+        <v>154.4</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="J86" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="L86" s="2">
+        <v>1</v>
+      </c>
+      <c r="M86" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="N86" s="2">
+        <v>1</v>
+      </c>
+      <c r="O86" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C87" s="2">
+        <v>78.2</v>
+      </c>
+      <c r="D87" s="2">
+        <v>155.6</v>
+      </c>
+      <c r="E87" s="2">
+        <v>208.1</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="J87" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="L87" s="2">
+        <v>1</v>
+      </c>
+      <c r="M87" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="N87" s="2">
+        <v>1</v>
+      </c>
+      <c r="O87" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="C88" s="3">
+        <v>235</v>
+      </c>
+      <c r="D88" s="3">
+        <v>76.3</v>
+      </c>
+      <c r="E88" s="3">
+        <v>137</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="L88" s="3">
+        <v>1</v>
+      </c>
+      <c r="M88" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="N88" s="3">
+        <v>1</v>
+      </c>
+      <c r="O88" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="C89" s="3">
+        <v>252.4</v>
+      </c>
+      <c r="D89" s="3">
+        <v>93.6</v>
+      </c>
+      <c r="E89" s="3">
+        <v>154.30000000000001</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="L89" s="3">
+        <v>1</v>
+      </c>
+      <c r="M89" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="N89" s="3">
+        <v>1</v>
+      </c>
+      <c r="O89" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="C90" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D90" s="3">
+        <v>196.2</v>
+      </c>
+      <c r="E90" s="3">
+        <v>257.2</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="L90" s="3">
+        <v>1</v>
+      </c>
+      <c r="M90" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="N90" s="3">
+        <v>1</v>
+      </c>
+      <c r="O90" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="C91" s="3">
+        <v>57.7</v>
+      </c>
+      <c r="D91" s="3">
+        <v>251.2</v>
+      </c>
+      <c r="E91" s="3">
+        <v>312.2</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="L91" s="3">
+        <v>1</v>
+      </c>
+      <c r="M91" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="N91" s="3">
+        <v>1</v>
+      </c>
+      <c r="O91" s="3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C92" s="3">
+        <v>78.5</v>
+      </c>
+      <c r="D92" s="3">
+        <v>271.8</v>
+      </c>
+      <c r="E92" s="3">
+        <v>332.8</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="L92" s="3">
+        <v>1</v>
+      </c>
+      <c r="M92" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="N92" s="3">
+        <v>1</v>
+      </c>
+      <c r="O92" s="3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="C93" s="3">
+        <v>199.9</v>
+      </c>
+      <c r="D93" s="3">
+        <v>25.9</v>
+      </c>
+      <c r="E93" s="3">
+        <v>87.1</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J93" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K93" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="L93" s="3">
+        <v>1</v>
+      </c>
+      <c r="M93" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="N93" s="3">
+        <v>1</v>
+      </c>
+      <c r="O93" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="C94" s="3">
+        <v>216.1</v>
+      </c>
+      <c r="D94" s="3">
+        <v>41.9</v>
+      </c>
+      <c r="E94" s="3">
+        <v>103.2</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J94" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K94" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="L94" s="3">
+        <v>1</v>
+      </c>
+      <c r="M94" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="N94" s="3">
+        <v>1</v>
+      </c>
+      <c r="O94" s="3" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="C95" s="3">
+        <v>152</v>
+      </c>
+      <c r="D95" s="3">
+        <v>322.8</v>
+      </c>
+      <c r="E95" s="3">
+        <v>24.6</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J95" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K95" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="L95" s="3">
+        <v>1</v>
+      </c>
+      <c r="M95" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="N95" s="3">
+        <v>1</v>
+      </c>
+      <c r="O95" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="C96" s="3">
+        <v>190</v>
+      </c>
+      <c r="D96" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E96" s="3">
+        <v>62.3</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J96" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K96" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="L96" s="3">
+        <v>1</v>
+      </c>
+      <c r="M96" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="N96" s="3">
+        <v>1</v>
+      </c>
+      <c r="O96" s="3" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>501</v>
+      </c>
+      <c r="B97" t="s">
+        <v>502</v>
+      </c>
+      <c r="C97" s="18">
+        <v>84.5</v>
+      </c>
+      <c r="D97">
+        <v>118.1</v>
+      </c>
+      <c r="E97">
+        <v>184.7</v>
+      </c>
+      <c r="F97" t="s">
+        <v>26</v>
+      </c>
+      <c r="G97" t="s">
+        <v>18</v>
+      </c>
+      <c r="H97" t="s">
+        <v>27</v>
+      </c>
+      <c r="I97" t="s">
+        <v>70</v>
+      </c>
+      <c r="J97" t="s">
+        <v>70</v>
+      </c>
+      <c r="K97" t="s">
+        <v>503</v>
+      </c>
+      <c r="L97">
+        <v>1</v>
+      </c>
+      <c r="M97" t="s">
+        <v>504</v>
+      </c>
+      <c r="N97">
+        <v>1</v>
+      </c>
+      <c r="O97" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>506</v>
+      </c>
+      <c r="B98" t="s">
+        <v>507</v>
+      </c>
+      <c r="C98" s="18">
+        <v>100.5</v>
+      </c>
+      <c r="D98">
+        <v>134</v>
+      </c>
+      <c r="E98">
+        <v>200.6</v>
+      </c>
+      <c r="F98" t="s">
+        <v>26</v>
+      </c>
+      <c r="G98" t="s">
+        <v>18</v>
+      </c>
+      <c r="H98" t="s">
+        <v>27</v>
+      </c>
+      <c r="I98" t="s">
+        <v>70</v>
+      </c>
+      <c r="J98" t="s">
+        <v>70</v>
+      </c>
+      <c r="K98" t="s">
+        <v>508</v>
+      </c>
+      <c r="L98">
+        <v>1</v>
+      </c>
+      <c r="M98" t="s">
+        <v>509</v>
+      </c>
+      <c r="N98">
+        <v>1</v>
+      </c>
+      <c r="O98" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="B99" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="C99" s="20">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="D99" s="19">
+        <v>45.9</v>
+      </c>
+      <c r="E99" s="19">
+        <v>114.9</v>
+      </c>
+      <c r="F99" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G99" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H99" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I99" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J99" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="K99" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="L99" s="19">
+        <v>1</v>
+      </c>
+      <c r="M99" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="N99" s="19">
+        <v>1</v>
+      </c>
+      <c r="O99" s="19" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="19" t="s">
+        <v>516</v>
+      </c>
+      <c r="B100" s="19" t="s">
+        <v>517</v>
+      </c>
+      <c r="C100" s="20">
+        <v>96.9</v>
+      </c>
+      <c r="D100" s="19">
+        <v>61.6</v>
+      </c>
+      <c r="E100" s="19">
+        <v>130.6</v>
+      </c>
+      <c r="F100" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G100" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H100" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I100" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J100" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="K100" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="L100" s="19">
+        <v>1</v>
+      </c>
+      <c r="M100" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="N100" s="19">
+        <v>1</v>
+      </c>
+      <c r="O100" s="19" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="B101" s="19" t="s">
+        <v>522</v>
+      </c>
+      <c r="C101" s="19">
+        <v>233.1</v>
+      </c>
+      <c r="D101" s="19">
+        <v>190.4</v>
+      </c>
+      <c r="E101" s="19">
+        <v>259.7</v>
+      </c>
+      <c r="F101" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G101" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H101" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I101" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J101" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="K101" s="19" t="s">
+        <v>523</v>
+      </c>
+      <c r="L101" s="19">
+        <v>1</v>
+      </c>
+      <c r="M101" s="19" t="s">
+        <v>524</v>
+      </c>
+      <c r="N101" s="19">
+        <v>1</v>
+      </c>
+      <c r="O101" s="19" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="B102" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="C102" s="19">
+        <v>249</v>
+      </c>
+      <c r="D102" s="19">
+        <v>206.1</v>
+      </c>
+      <c r="E102" s="19">
+        <v>275.39999999999998</v>
+      </c>
+      <c r="F102" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G102" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H102" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="J102" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="K102" s="19" t="s">
+        <v>528</v>
+      </c>
+      <c r="L102" s="19">
+        <v>1</v>
+      </c>
+      <c r="M102" s="19" t="s">
+        <v>529</v>
+      </c>
+      <c r="N102" s="19">
+        <v>1</v>
+      </c>
+      <c r="O102" s="19" t="s">
+        <v>530</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O78" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter val="2023*"/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <customFilters and="1">
-        <customFilter operator="greaterThanOrEqual" val="35"/>
-        <customFilter operator="lessThanOrEqual" val="55"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O100" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final ESS Paper submission
Includes effort to 'debug' weighting functions and transmissions for a purely absorbing atmosphere. A few updates to plotting routines. And also a bit of work on results versus airmass
</commit_message>
<xml_diff>
--- a/Catalog/Catalog-static.xlsx
+++ b/Catalog/Catalog-static.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BF02F5-55D3-4DDE-811F-6F7A0C44EC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF62F0EC-2203-4430-8B3A-1FD1DA7E90AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2546,7 +2546,7 @@
   <dimension ref="A1:O102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="D99" sqref="D99"/>

</xml_diff>

<commit_message>
Gravity, eta=2, reprocessing, Europlanet webinar, size
Moved all base data products (L2, L3, Plots, Images) outside of the repo since it had grown too large for GitHub. Also, added latitude dependent gravity and used eta=2 per Irwin et al., 2025. Then I updated and improved scripts and reprocessed all the data. I improved some codes and produced the charts and analyses for the Europlanet webinar on Feb. 28, 2025. Finally, I moved all the base data (L2, L3, Map plots, and images) out of the repo since it had gotten too large for GitHub.
</commit_message>
<xml_diff>
--- a/Catalog/Catalog-static.xlsx
+++ b/Catalog/Catalog-static.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB2823A-D022-4851-8477-9D4C238C83CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC1A8AF-5D78-4E87-8AA5-5A719AA76F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="380" windowWidth="19180" windowHeight="9700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalog-static" sheetId="1" r:id="rId1"/>
     <sheet name="Status &amp; Notes" sheetId="3" r:id="rId2"/>
     <sheet name="Related Missions &amp; Observations" sheetId="2" r:id="rId3"/>
+    <sheet name="Scratch" sheetId="4" r:id="rId4"/>
+    <sheet name="Validation" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Catalog-static'!$A$1:$O$102</definedName>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="927">
   <si>
     <t>ObsID</t>
   </si>
@@ -2116,6 +2118,732 @@
   </si>
   <si>
     <t>2024-10-22-1225_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Maybe some striping on early sequences?</t>
+  </si>
+  <si>
+    <t>Lots of high clouds, poor quality.</t>
+  </si>
+  <si>
+    <t>Proc. Status</t>
+  </si>
+  <si>
+    <t>Zipped</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>Archive</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Processed</t>
+  </si>
+  <si>
+    <t>Archive Status</t>
+  </si>
+  <si>
+    <t>Possible obscuration on later sequences due to trees</t>
+  </si>
+  <si>
+    <t>20241023UTa</t>
+  </si>
+  <si>
+    <t>2024-10-23_04:53:24</t>
+  </si>
+  <si>
+    <t>2024-10-23-0453_4-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-23-0453_4-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-23-0505_6-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241027UTa</t>
+  </si>
+  <si>
+    <t>2024-10-27_05:13:06</t>
+  </si>
+  <si>
+    <t>2024-10-27-0513_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0513_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0523_6-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241027UTb</t>
+  </si>
+  <si>
+    <t>2024-10-27_05:34:06</t>
+  </si>
+  <si>
+    <t>2024-10-27-0534_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0534_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0608_6-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241027UTc</t>
+  </si>
+  <si>
+    <t>2024-10-27_05:58:06</t>
+  </si>
+  <si>
+    <t>2024-10-27-0558_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0558_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>20241027UTd</t>
+  </si>
+  <si>
+    <t>2024-10-27_06:19:06</t>
+  </si>
+  <si>
+    <t>2024-10-27-0619_0-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0619_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0629_6-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241027UTe</t>
+  </si>
+  <si>
+    <t>2024-10-27_06:50:42</t>
+  </si>
+  <si>
+    <t>2024-10-27-0650_8-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0650_7-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0701_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241027UTf</t>
+  </si>
+  <si>
+    <t>2024-10-27_07:11:42</t>
+  </si>
+  <si>
+    <t>2024-10-27-0711_7-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0711_7-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0722_2-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241027UTg</t>
+  </si>
+  <si>
+    <t>2024-10-27_07:46:48</t>
+  </si>
+  <si>
+    <t>2024-10-27-0746_8-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0746_8-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0757_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241027UTh</t>
+  </si>
+  <si>
+    <t>2024-10-27_08:07:48</t>
+  </si>
+  <si>
+    <t>2024-10-27-0807_8-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0807_8-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0818_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241027UTi</t>
+  </si>
+  <si>
+    <t>2024-10-27_08:49:18</t>
+  </si>
+  <si>
+    <t>2024-10-27-0849_3-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0859_8-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241027UTj</t>
+  </si>
+  <si>
+    <t>2024-10-27_09:10:18</t>
+  </si>
+  <si>
+    <t>2024-10-27-0910_3-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0910_3-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-10-27-0920_8-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241105UTf</t>
+  </si>
+  <si>
+    <t>2024-11-05_07:16:06</t>
+  </si>
+  <si>
+    <t>2024-11-05-0716_2-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-05-0716_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-05-0726_6-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241115UTa</t>
+  </si>
+  <si>
+    <t>2024-11-15_04:35:24</t>
+  </si>
+  <si>
+    <t>2024-11-15-0435_4-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0435_4-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0445_9-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241115UTb</t>
+  </si>
+  <si>
+    <t>2024-11-15_04:56:18</t>
+  </si>
+  <si>
+    <t>2024-11-15-0456_3-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0456_3-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0506_8-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241115UTc</t>
+  </si>
+  <si>
+    <t>2024-11-15_05:17:12</t>
+  </si>
+  <si>
+    <t>2024-11-15-0517_3-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0517_2-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0527_7-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241115UTd</t>
+  </si>
+  <si>
+    <t>2024-11-15_05:38:06</t>
+  </si>
+  <si>
+    <t>2024-11-15-0538_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0538_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0548_6-Jupiter_R685G550B632450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241115UTe</t>
+  </si>
+  <si>
+    <t>2024-11-15_06:06:12</t>
+  </si>
+  <si>
+    <t>2024-11-15-0606_2-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0606_2-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0616_7-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241115UTf</t>
+  </si>
+  <si>
+    <t>2024-11-15_06:27:06</t>
+  </si>
+  <si>
+    <t>2024-11-15-0627_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0627_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0637_6-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241115UTg</t>
+  </si>
+  <si>
+    <t>2024-11-15_06:48:00</t>
+  </si>
+  <si>
+    <t>2024-11-15-0648_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0648_0-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0658_5-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241115UTh</t>
+  </si>
+  <si>
+    <t>2024-11-15_07:09:00</t>
+  </si>
+  <si>
+    <t>2024-11-15-0708_9-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0709_0-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0719_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241115UTi</t>
+  </si>
+  <si>
+    <t>2024-11-15_07:29:54</t>
+  </si>
+  <si>
+    <t>2024-11-15-0729_9-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0729_9-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-15-0740_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTa</t>
+  </si>
+  <si>
+    <t>2024-11-29_03:36:18</t>
+  </si>
+  <si>
+    <t>2024-11-29-0336_3-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0336_3-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0346_8-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTb</t>
+  </si>
+  <si>
+    <t>2024-11-29_03:56:54</t>
+  </si>
+  <si>
+    <t>2024-11-29-0357_2-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0356_9-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0407_7-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTc</t>
+  </si>
+  <si>
+    <t>2024-11-29_04:18:06</t>
+  </si>
+  <si>
+    <t>2024-11-29-0418_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0418_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0428_6-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTd</t>
+  </si>
+  <si>
+    <t>2024-11-29_04:39:00</t>
+  </si>
+  <si>
+    <t>2024-11-29-0439_0-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0449_5-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTe</t>
+  </si>
+  <si>
+    <t>2024-11-29_05:00:00</t>
+  </si>
+  <si>
+    <t>2024-11-29-0459_9-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0500_0-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0510_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTf</t>
+  </si>
+  <si>
+    <t>2024-11-29_05:20:54</t>
+  </si>
+  <si>
+    <t>2024-11-29-0520_9-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0520_9-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0531_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTg</t>
+  </si>
+  <si>
+    <t>2024-11-29_05:41:48</t>
+  </si>
+  <si>
+    <t>2024-11-29-0541_8-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0541_8-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0552_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTh</t>
+  </si>
+  <si>
+    <t>2024-11-29_06:02:42</t>
+  </si>
+  <si>
+    <t>2024-11-29-0602_8-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0602_7-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0613_2-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTi</t>
+  </si>
+  <si>
+    <t>2024-11-29_06:26:36</t>
+  </si>
+  <si>
+    <t>2024-11-29-0626_6-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0626_6-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0637_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTj</t>
+  </si>
+  <si>
+    <t>2024-11-29_06:47:36</t>
+  </si>
+  <si>
+    <t>2024-11-29-0647_6-Jupiter_R665G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0647_6-Jupiter_R665G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0658_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTk</t>
+  </si>
+  <si>
+    <t>2024-11-29_07:08:30</t>
+  </si>
+  <si>
+    <t>2024-11-29-0708_5-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0708_5-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0719_0-Jupiter_R686G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTl</t>
+  </si>
+  <si>
+    <t>2024-11-29_07:29:24</t>
+  </si>
+  <si>
+    <t>2024-11-29-0729_4-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0729_4-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0739_9-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTm</t>
+  </si>
+  <si>
+    <t>2024-11-29_07:50:18</t>
+  </si>
+  <si>
+    <t>2024-11-29-0750_4-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0750_3-Jupiter_R656G647B632-RGB_WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0800_8-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241129UTn</t>
+  </si>
+  <si>
+    <t>2024-11-29_08:11:18</t>
+  </si>
+  <si>
+    <t>2024-11-29-0811_3-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-11-29-0811_3-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>20241202UTa</t>
+  </si>
+  <si>
+    <t>2024-12-02_02:51:36</t>
+  </si>
+  <si>
+    <t>2024-12-02-0251_6-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0251_6-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0302_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241202UTb</t>
+  </si>
+  <si>
+    <t>2024-12-02_03:12:30</t>
+  </si>
+  <si>
+    <t>2024-12-02-0312_5-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0312_5-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0323_0-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241202UTc</t>
+  </si>
+  <si>
+    <t>2024-12-02_03:33:24</t>
+  </si>
+  <si>
+    <t>2024-12-02-0333_5-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0333_4-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0343_9-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241202UTd</t>
+  </si>
+  <si>
+    <t>2024-12-02_03:55:48</t>
+  </si>
+  <si>
+    <t>2024-12-02-0355_8-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0355_8-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0406_2-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241202UTe</t>
+  </si>
+  <si>
+    <t>2024-12-02_04:16:42</t>
+  </si>
+  <si>
+    <t>2024-12-02-0416_7-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0416_7-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0427_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241202UTf</t>
+  </si>
+  <si>
+    <t>2024-12-02_04:37:36</t>
+  </si>
+  <si>
+    <t>2024-12-02-0437_6-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0437_6-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0448_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241202UTg</t>
+  </si>
+  <si>
+    <t>2024-12-02_04:58:30</t>
+  </si>
+  <si>
+    <t>2024-12-02-0458_5-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0458_5-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0509_0-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20241202UTh</t>
+  </si>
+  <si>
+    <t>2024-12-02_05:19:24</t>
+  </si>
+  <si>
+    <t>2024-12-02-0519_4-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0519_4-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2024-12-02-0529_9-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>Good NEDFs (240-360), Good SEB outbreak</t>
+  </si>
+  <si>
+    <t>Possible obscuration on later sequences due to trees; 1/28 00:43 has some of the tail of the NTB outbreak</t>
+  </si>
+  <si>
+    <t>?? is this 16?</t>
+  </si>
+  <si>
+    <t>Stacked</t>
+  </si>
+  <si>
+    <t>Good NEDFs (240-360), Good GRS</t>
+  </si>
+  <si>
+    <t>Poor focus</t>
+  </si>
+  <si>
+    <t>Very good focus, Good GRS</t>
+  </si>
+  <si>
+    <t>Flats! Poor to very good focus, Good GRS, Good SEB outbreak</t>
+  </si>
+  <si>
+    <t>Good to very good focus, Good GRS, Good SEB outbreak, Good NTB outbreak</t>
+  </si>
+  <si>
+    <t>Poor focus, Maybe some good NEDFs</t>
+  </si>
+  <si>
+    <t>L1~15-240 NEDF coverage</t>
+  </si>
+  <si>
+    <t>L1~0-230 NEDF coverage</t>
+  </si>
+  <si>
+    <t>L1~110-310 NEDF coverage</t>
+  </si>
+  <si>
+    <t>Very good focus, Good GRS - Seems like 15 Sci and 14 RGB</t>
+  </si>
+  <si>
+    <t>Very good focus, Good SEB outbreak, Good GRS(only 16 RGB) Plus 2 RGB 1x1 sets</t>
+  </si>
+  <si>
+    <t>Leigh VISIER Data</t>
   </si>
 </sst>
 </file>
@@ -2703,7 +3431,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -2746,6 +3474,8 @@
     <xf numFmtId="0" fontId="21" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3101,20 +3831,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O129"/>
+  <dimension ref="A1:O177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D96" sqref="D96"/>
+      <selection pane="bottomRight" activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.81640625" customWidth="1"/>
     <col min="2" max="2" width="27.26953125" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" customWidth="1"/>
     <col min="8" max="8" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9179,6 +9909,2027 @@
       </c>
       <c r="O129" t="s">
         <v>684</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>700</v>
+      </c>
+      <c r="B130" t="s">
+        <v>701</v>
+      </c>
+      <c r="C130">
+        <v>133.19999999999999</v>
+      </c>
+      <c r="D130">
+        <v>88.8</v>
+      </c>
+      <c r="E130">
+        <v>220.9</v>
+      </c>
+      <c r="F130" t="s">
+        <v>26</v>
+      </c>
+      <c r="G130" t="s">
+        <v>18</v>
+      </c>
+      <c r="H130" t="s">
+        <v>27</v>
+      </c>
+      <c r="I130" t="s">
+        <v>610</v>
+      </c>
+      <c r="J130" t="s">
+        <v>610</v>
+      </c>
+      <c r="K130" t="s">
+        <v>702</v>
+      </c>
+      <c r="L130">
+        <v>1</v>
+      </c>
+      <c r="M130" t="s">
+        <v>703</v>
+      </c>
+      <c r="N130">
+        <v>1</v>
+      </c>
+      <c r="O130" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>705</v>
+      </c>
+      <c r="B131" t="s">
+        <v>706</v>
+      </c>
+      <c r="C131">
+        <v>57.2</v>
+      </c>
+      <c r="D131">
+        <v>342.2</v>
+      </c>
+      <c r="E131">
+        <v>115.3</v>
+      </c>
+      <c r="F131" t="s">
+        <v>26</v>
+      </c>
+      <c r="G131" t="s">
+        <v>18</v>
+      </c>
+      <c r="H131" t="s">
+        <v>27</v>
+      </c>
+      <c r="I131" t="s">
+        <v>610</v>
+      </c>
+      <c r="J131" t="s">
+        <v>610</v>
+      </c>
+      <c r="K131" t="s">
+        <v>707</v>
+      </c>
+      <c r="L131">
+        <v>1</v>
+      </c>
+      <c r="M131" t="s">
+        <v>708</v>
+      </c>
+      <c r="N131">
+        <v>1</v>
+      </c>
+      <c r="O131" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>710</v>
+      </c>
+      <c r="B132" t="s">
+        <v>711</v>
+      </c>
+      <c r="C132">
+        <v>70</v>
+      </c>
+      <c r="D132">
+        <v>354.9</v>
+      </c>
+      <c r="E132">
+        <v>128</v>
+      </c>
+      <c r="F132" t="s">
+        <v>26</v>
+      </c>
+      <c r="G132" t="s">
+        <v>18</v>
+      </c>
+      <c r="H132" t="s">
+        <v>27</v>
+      </c>
+      <c r="I132" t="s">
+        <v>610</v>
+      </c>
+      <c r="J132" t="s">
+        <v>610</v>
+      </c>
+      <c r="K132" t="s">
+        <v>712</v>
+      </c>
+      <c r="L132">
+        <v>1</v>
+      </c>
+      <c r="M132" t="s">
+        <v>713</v>
+      </c>
+      <c r="N132">
+        <v>1</v>
+      </c>
+      <c r="O132" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>715</v>
+      </c>
+      <c r="B133" t="s">
+        <v>716</v>
+      </c>
+      <c r="C133">
+        <v>84.7</v>
+      </c>
+      <c r="D133">
+        <v>9.4</v>
+      </c>
+      <c r="E133">
+        <v>142.5</v>
+      </c>
+      <c r="F133" t="s">
+        <v>26</v>
+      </c>
+      <c r="G133" t="s">
+        <v>18</v>
+      </c>
+      <c r="H133" t="s">
+        <v>27</v>
+      </c>
+      <c r="I133" t="s">
+        <v>610</v>
+      </c>
+      <c r="J133" t="s">
+        <v>610</v>
+      </c>
+      <c r="K133" t="s">
+        <v>717</v>
+      </c>
+      <c r="L133">
+        <v>1</v>
+      </c>
+      <c r="M133" t="s">
+        <v>718</v>
+      </c>
+      <c r="N133">
+        <v>1</v>
+      </c>
+      <c r="O133" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>719</v>
+      </c>
+      <c r="B134" t="s">
+        <v>720</v>
+      </c>
+      <c r="C134">
+        <v>97.5</v>
+      </c>
+      <c r="D134">
+        <v>22.1</v>
+      </c>
+      <c r="E134">
+        <v>155.19999999999999</v>
+      </c>
+      <c r="F134" t="s">
+        <v>26</v>
+      </c>
+      <c r="G134" t="s">
+        <v>18</v>
+      </c>
+      <c r="H134" t="s">
+        <v>27</v>
+      </c>
+      <c r="I134" t="s">
+        <v>610</v>
+      </c>
+      <c r="J134" t="s">
+        <v>610</v>
+      </c>
+      <c r="K134" t="s">
+        <v>721</v>
+      </c>
+      <c r="L134">
+        <v>1</v>
+      </c>
+      <c r="M134" t="s">
+        <v>722</v>
+      </c>
+      <c r="N134">
+        <v>1</v>
+      </c>
+      <c r="O134" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>724</v>
+      </c>
+      <c r="B135" t="s">
+        <v>725</v>
+      </c>
+      <c r="C135">
+        <v>116.8</v>
+      </c>
+      <c r="D135">
+        <v>41.2</v>
+      </c>
+      <c r="E135">
+        <v>174.3</v>
+      </c>
+      <c r="F135" t="s">
+        <v>26</v>
+      </c>
+      <c r="G135" t="s">
+        <v>18</v>
+      </c>
+      <c r="H135" t="s">
+        <v>27</v>
+      </c>
+      <c r="I135" t="s">
+        <v>610</v>
+      </c>
+      <c r="J135" t="s">
+        <v>610</v>
+      </c>
+      <c r="K135" t="s">
+        <v>726</v>
+      </c>
+      <c r="L135">
+        <v>1</v>
+      </c>
+      <c r="M135" t="s">
+        <v>727</v>
+      </c>
+      <c r="N135">
+        <v>1</v>
+      </c>
+      <c r="O135" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>729</v>
+      </c>
+      <c r="B136" t="s">
+        <v>730</v>
+      </c>
+      <c r="C136">
+        <v>129.6</v>
+      </c>
+      <c r="D136">
+        <v>53.9</v>
+      </c>
+      <c r="E136">
+        <v>187</v>
+      </c>
+      <c r="F136" t="s">
+        <v>26</v>
+      </c>
+      <c r="G136" t="s">
+        <v>18</v>
+      </c>
+      <c r="H136" t="s">
+        <v>27</v>
+      </c>
+      <c r="I136" t="s">
+        <v>610</v>
+      </c>
+      <c r="J136" t="s">
+        <v>610</v>
+      </c>
+      <c r="K136" t="s">
+        <v>731</v>
+      </c>
+      <c r="L136">
+        <v>1</v>
+      </c>
+      <c r="M136" t="s">
+        <v>732</v>
+      </c>
+      <c r="N136">
+        <v>1</v>
+      </c>
+      <c r="O136" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>734</v>
+      </c>
+      <c r="B137" t="s">
+        <v>735</v>
+      </c>
+      <c r="C137">
+        <v>151</v>
+      </c>
+      <c r="D137">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="E137">
+        <v>208.3</v>
+      </c>
+      <c r="F137" t="s">
+        <v>26</v>
+      </c>
+      <c r="G137" t="s">
+        <v>18</v>
+      </c>
+      <c r="H137" t="s">
+        <v>27</v>
+      </c>
+      <c r="I137" t="s">
+        <v>610</v>
+      </c>
+      <c r="J137" t="s">
+        <v>610</v>
+      </c>
+      <c r="K137" t="s">
+        <v>736</v>
+      </c>
+      <c r="L137">
+        <v>1</v>
+      </c>
+      <c r="M137" t="s">
+        <v>737</v>
+      </c>
+      <c r="N137">
+        <v>1</v>
+      </c>
+      <c r="O137" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>739</v>
+      </c>
+      <c r="B138" t="s">
+        <v>740</v>
+      </c>
+      <c r="C138">
+        <v>163.80000000000001</v>
+      </c>
+      <c r="D138">
+        <v>87.8</v>
+      </c>
+      <c r="E138">
+        <v>221</v>
+      </c>
+      <c r="F138" t="s">
+        <v>26</v>
+      </c>
+      <c r="G138" t="s">
+        <v>18</v>
+      </c>
+      <c r="H138" t="s">
+        <v>27</v>
+      </c>
+      <c r="I138" t="s">
+        <v>610</v>
+      </c>
+      <c r="J138" t="s">
+        <v>610</v>
+      </c>
+      <c r="K138" t="s">
+        <v>741</v>
+      </c>
+      <c r="L138">
+        <v>1</v>
+      </c>
+      <c r="M138" t="s">
+        <v>742</v>
+      </c>
+      <c r="N138">
+        <v>1</v>
+      </c>
+      <c r="O138" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>744</v>
+      </c>
+      <c r="B139" t="s">
+        <v>745</v>
+      </c>
+      <c r="C139">
+        <v>189.1</v>
+      </c>
+      <c r="D139">
+        <v>112.9</v>
+      </c>
+      <c r="E139">
+        <v>246</v>
+      </c>
+      <c r="F139" t="s">
+        <v>26</v>
+      </c>
+      <c r="G139" t="s">
+        <v>18</v>
+      </c>
+      <c r="H139" t="s">
+        <v>27</v>
+      </c>
+      <c r="I139" t="s">
+        <v>610</v>
+      </c>
+      <c r="J139" t="s">
+        <v>610</v>
+      </c>
+      <c r="K139" t="s">
+        <v>746</v>
+      </c>
+      <c r="L139">
+        <v>1</v>
+      </c>
+      <c r="M139" t="s">
+        <v>746</v>
+      </c>
+      <c r="N139">
+        <v>1</v>
+      </c>
+      <c r="O139" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>748</v>
+      </c>
+      <c r="B140" t="s">
+        <v>749</v>
+      </c>
+      <c r="C140">
+        <v>201.9</v>
+      </c>
+      <c r="D140">
+        <v>125.6</v>
+      </c>
+      <c r="E140">
+        <v>258.7</v>
+      </c>
+      <c r="F140" t="s">
+        <v>26</v>
+      </c>
+      <c r="G140" t="s">
+        <v>18</v>
+      </c>
+      <c r="H140" t="s">
+        <v>27</v>
+      </c>
+      <c r="I140" t="s">
+        <v>610</v>
+      </c>
+      <c r="J140" t="s">
+        <v>610</v>
+      </c>
+      <c r="K140" t="s">
+        <v>750</v>
+      </c>
+      <c r="L140">
+        <v>1</v>
+      </c>
+      <c r="M140" t="s">
+        <v>751</v>
+      </c>
+      <c r="N140">
+        <v>1</v>
+      </c>
+      <c r="O140" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>753</v>
+      </c>
+      <c r="B146" t="s">
+        <v>754</v>
+      </c>
+      <c r="C146">
+        <v>114.4</v>
+      </c>
+      <c r="D146">
+        <v>330</v>
+      </c>
+      <c r="E146">
+        <v>105.5</v>
+      </c>
+      <c r="F146" t="s">
+        <v>26</v>
+      </c>
+      <c r="G146" t="s">
+        <v>18</v>
+      </c>
+      <c r="H146" t="s">
+        <v>27</v>
+      </c>
+      <c r="I146" t="s">
+        <v>132</v>
+      </c>
+      <c r="J146" t="s">
+        <v>70</v>
+      </c>
+      <c r="K146" t="s">
+        <v>755</v>
+      </c>
+      <c r="L146">
+        <v>1</v>
+      </c>
+      <c r="M146" t="s">
+        <v>756</v>
+      </c>
+      <c r="N146">
+        <v>1</v>
+      </c>
+      <c r="O146" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>758</v>
+      </c>
+      <c r="B147" t="s">
+        <v>759</v>
+      </c>
+      <c r="C147">
+        <v>156.69999999999999</v>
+      </c>
+      <c r="D147">
+        <v>296.8</v>
+      </c>
+      <c r="E147">
+        <v>75</v>
+      </c>
+      <c r="F147" t="s">
+        <v>26</v>
+      </c>
+      <c r="G147" t="s">
+        <v>18</v>
+      </c>
+      <c r="H147" t="s">
+        <v>27</v>
+      </c>
+      <c r="I147" t="s">
+        <v>132</v>
+      </c>
+      <c r="J147" t="s">
+        <v>70</v>
+      </c>
+      <c r="K147" t="s">
+        <v>760</v>
+      </c>
+      <c r="L147">
+        <v>1</v>
+      </c>
+      <c r="M147" t="s">
+        <v>761</v>
+      </c>
+      <c r="N147">
+        <v>1</v>
+      </c>
+      <c r="O147" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>763</v>
+      </c>
+      <c r="B148" t="s">
+        <v>764</v>
+      </c>
+      <c r="C148">
+        <v>169.4</v>
+      </c>
+      <c r="D148">
+        <v>309.5</v>
+      </c>
+      <c r="E148">
+        <v>87.7</v>
+      </c>
+      <c r="F148" t="s">
+        <v>26</v>
+      </c>
+      <c r="G148" t="s">
+        <v>18</v>
+      </c>
+      <c r="H148" t="s">
+        <v>27</v>
+      </c>
+      <c r="I148" t="s">
+        <v>132</v>
+      </c>
+      <c r="J148" t="s">
+        <v>70</v>
+      </c>
+      <c r="K148" t="s">
+        <v>765</v>
+      </c>
+      <c r="L148">
+        <v>1</v>
+      </c>
+      <c r="M148" t="s">
+        <v>766</v>
+      </c>
+      <c r="N148">
+        <v>1</v>
+      </c>
+      <c r="O148" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>768</v>
+      </c>
+      <c r="B149" t="s">
+        <v>769</v>
+      </c>
+      <c r="C149">
+        <v>182.2</v>
+      </c>
+      <c r="D149">
+        <v>322.10000000000002</v>
+      </c>
+      <c r="E149">
+        <v>100.3</v>
+      </c>
+      <c r="F149" t="s">
+        <v>26</v>
+      </c>
+      <c r="G149" t="s">
+        <v>18</v>
+      </c>
+      <c r="H149" t="s">
+        <v>27</v>
+      </c>
+      <c r="I149" t="s">
+        <v>132</v>
+      </c>
+      <c r="J149" t="s">
+        <v>70</v>
+      </c>
+      <c r="K149" t="s">
+        <v>770</v>
+      </c>
+      <c r="L149">
+        <v>1</v>
+      </c>
+      <c r="M149" t="s">
+        <v>771</v>
+      </c>
+      <c r="N149">
+        <v>1</v>
+      </c>
+      <c r="O149" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
+        <v>773</v>
+      </c>
+      <c r="B150" t="s">
+        <v>774</v>
+      </c>
+      <c r="C150">
+        <v>194.9</v>
+      </c>
+      <c r="D150">
+        <v>334.7</v>
+      </c>
+      <c r="E150">
+        <v>112.9</v>
+      </c>
+      <c r="F150" t="s">
+        <v>26</v>
+      </c>
+      <c r="G150" t="s">
+        <v>18</v>
+      </c>
+      <c r="H150" t="s">
+        <v>27</v>
+      </c>
+      <c r="I150" t="s">
+        <v>132</v>
+      </c>
+      <c r="J150" t="s">
+        <v>70</v>
+      </c>
+      <c r="K150" t="s">
+        <v>775</v>
+      </c>
+      <c r="L150">
+        <v>1</v>
+      </c>
+      <c r="M150" t="s">
+        <v>776</v>
+      </c>
+      <c r="N150">
+        <v>1</v>
+      </c>
+      <c r="O150" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>778</v>
+      </c>
+      <c r="B151" t="s">
+        <v>779</v>
+      </c>
+      <c r="C151">
+        <v>212</v>
+      </c>
+      <c r="D151">
+        <v>351.7</v>
+      </c>
+      <c r="E151">
+        <v>129.9</v>
+      </c>
+      <c r="F151" t="s">
+        <v>26</v>
+      </c>
+      <c r="G151" t="s">
+        <v>18</v>
+      </c>
+      <c r="H151" t="s">
+        <v>27</v>
+      </c>
+      <c r="I151" t="s">
+        <v>132</v>
+      </c>
+      <c r="J151" t="s">
+        <v>70</v>
+      </c>
+      <c r="K151" t="s">
+        <v>780</v>
+      </c>
+      <c r="L151">
+        <v>1</v>
+      </c>
+      <c r="M151" t="s">
+        <v>781</v>
+      </c>
+      <c r="N151">
+        <v>1</v>
+      </c>
+      <c r="O151" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>783</v>
+      </c>
+      <c r="B152" t="s">
+        <v>784</v>
+      </c>
+      <c r="C152">
+        <v>224.8</v>
+      </c>
+      <c r="D152">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E152">
+        <v>142.6</v>
+      </c>
+      <c r="F152" t="s">
+        <v>26</v>
+      </c>
+      <c r="G152" t="s">
+        <v>18</v>
+      </c>
+      <c r="H152" t="s">
+        <v>27</v>
+      </c>
+      <c r="I152" t="s">
+        <v>132</v>
+      </c>
+      <c r="J152" t="s">
+        <v>70</v>
+      </c>
+      <c r="K152" t="s">
+        <v>785</v>
+      </c>
+      <c r="L152">
+        <v>1</v>
+      </c>
+      <c r="M152" t="s">
+        <v>786</v>
+      </c>
+      <c r="N152">
+        <v>1</v>
+      </c>
+      <c r="O152" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>788</v>
+      </c>
+      <c r="B153" t="s">
+        <v>789</v>
+      </c>
+      <c r="C153">
+        <v>237.5</v>
+      </c>
+      <c r="D153">
+        <v>17</v>
+      </c>
+      <c r="E153">
+        <v>155.19999999999999</v>
+      </c>
+      <c r="F153" t="s">
+        <v>26</v>
+      </c>
+      <c r="G153" t="s">
+        <v>18</v>
+      </c>
+      <c r="H153" t="s">
+        <v>27</v>
+      </c>
+      <c r="I153" t="s">
+        <v>132</v>
+      </c>
+      <c r="J153" t="s">
+        <v>70</v>
+      </c>
+      <c r="K153" t="s">
+        <v>790</v>
+      </c>
+      <c r="L153">
+        <v>1</v>
+      </c>
+      <c r="M153" t="s">
+        <v>791</v>
+      </c>
+      <c r="N153">
+        <v>1</v>
+      </c>
+      <c r="O153" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>793</v>
+      </c>
+      <c r="B154" t="s">
+        <v>794</v>
+      </c>
+      <c r="C154">
+        <v>250.3</v>
+      </c>
+      <c r="D154">
+        <v>29.7</v>
+      </c>
+      <c r="E154">
+        <v>167.9</v>
+      </c>
+      <c r="F154" t="s">
+        <v>26</v>
+      </c>
+      <c r="G154" t="s">
+        <v>18</v>
+      </c>
+      <c r="H154" t="s">
+        <v>27</v>
+      </c>
+      <c r="I154" t="s">
+        <v>132</v>
+      </c>
+      <c r="J154" t="s">
+        <v>70</v>
+      </c>
+      <c r="K154" t="s">
+        <v>795</v>
+      </c>
+      <c r="L154">
+        <v>1</v>
+      </c>
+      <c r="M154" t="s">
+        <v>796</v>
+      </c>
+      <c r="N154">
+        <v>1</v>
+      </c>
+      <c r="O154" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>798</v>
+      </c>
+      <c r="B155" t="s">
+        <v>799</v>
+      </c>
+      <c r="C155">
+        <v>263.10000000000002</v>
+      </c>
+      <c r="D155">
+        <v>42.3</v>
+      </c>
+      <c r="E155">
+        <v>180.5</v>
+      </c>
+      <c r="F155" t="s">
+        <v>26</v>
+      </c>
+      <c r="G155" t="s">
+        <v>18</v>
+      </c>
+      <c r="H155" t="s">
+        <v>27</v>
+      </c>
+      <c r="I155" t="s">
+        <v>132</v>
+      </c>
+      <c r="J155" t="s">
+        <v>70</v>
+      </c>
+      <c r="K155" t="s">
+        <v>800</v>
+      </c>
+      <c r="L155">
+        <v>1</v>
+      </c>
+      <c r="M155" t="s">
+        <v>801</v>
+      </c>
+      <c r="N155">
+        <v>1</v>
+      </c>
+      <c r="O155" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>803</v>
+      </c>
+      <c r="B156" t="s">
+        <v>804</v>
+      </c>
+      <c r="C156">
+        <v>173.2</v>
+      </c>
+      <c r="D156">
+        <v>206.9</v>
+      </c>
+      <c r="E156">
+        <v>348.7</v>
+      </c>
+      <c r="F156" t="s">
+        <v>26</v>
+      </c>
+      <c r="G156" t="s">
+        <v>18</v>
+      </c>
+      <c r="H156" t="s">
+        <v>27</v>
+      </c>
+      <c r="I156" t="s">
+        <v>132</v>
+      </c>
+      <c r="J156" t="s">
+        <v>70</v>
+      </c>
+      <c r="K156" t="s">
+        <v>805</v>
+      </c>
+      <c r="L156">
+        <v>1</v>
+      </c>
+      <c r="M156" t="s">
+        <v>806</v>
+      </c>
+      <c r="N156">
+        <v>1</v>
+      </c>
+      <c r="O156" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>808</v>
+      </c>
+      <c r="B157" t="s">
+        <v>809</v>
+      </c>
+      <c r="C157">
+        <v>185.7</v>
+      </c>
+      <c r="D157">
+        <v>219.3</v>
+      </c>
+      <c r="E157">
+        <v>1.2</v>
+      </c>
+      <c r="F157" t="s">
+        <v>26</v>
+      </c>
+      <c r="G157" t="s">
+        <v>18</v>
+      </c>
+      <c r="H157" t="s">
+        <v>27</v>
+      </c>
+      <c r="I157" t="s">
+        <v>132</v>
+      </c>
+      <c r="J157" t="s">
+        <v>70</v>
+      </c>
+      <c r="K157" t="s">
+        <v>810</v>
+      </c>
+      <c r="L157">
+        <v>1</v>
+      </c>
+      <c r="M157" t="s">
+        <v>811</v>
+      </c>
+      <c r="N157">
+        <v>1</v>
+      </c>
+      <c r="O157" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>813</v>
+      </c>
+      <c r="B158" t="s">
+        <v>814</v>
+      </c>
+      <c r="C158">
+        <v>198.7</v>
+      </c>
+      <c r="D158">
+        <v>232.1</v>
+      </c>
+      <c r="E158">
+        <v>14</v>
+      </c>
+      <c r="F158" t="s">
+        <v>26</v>
+      </c>
+      <c r="G158" t="s">
+        <v>18</v>
+      </c>
+      <c r="H158" t="s">
+        <v>27</v>
+      </c>
+      <c r="I158" t="s">
+        <v>132</v>
+      </c>
+      <c r="J158" t="s">
+        <v>70</v>
+      </c>
+      <c r="K158" t="s">
+        <v>815</v>
+      </c>
+      <c r="L158">
+        <v>1</v>
+      </c>
+      <c r="M158" t="s">
+        <v>816</v>
+      </c>
+      <c r="N158">
+        <v>1</v>
+      </c>
+      <c r="O158" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>818</v>
+      </c>
+      <c r="B159" t="s">
+        <v>819</v>
+      </c>
+      <c r="C159">
+        <v>211.4</v>
+      </c>
+      <c r="D159">
+        <v>244.8</v>
+      </c>
+      <c r="E159">
+        <v>26.7</v>
+      </c>
+      <c r="F159" t="s">
+        <v>26</v>
+      </c>
+      <c r="G159" t="s">
+        <v>18</v>
+      </c>
+      <c r="H159" t="s">
+        <v>27</v>
+      </c>
+      <c r="I159" t="s">
+        <v>132</v>
+      </c>
+      <c r="J159" t="s">
+        <v>70</v>
+      </c>
+      <c r="K159" t="s">
+        <v>820</v>
+      </c>
+      <c r="L159">
+        <v>1</v>
+      </c>
+      <c r="M159" t="s">
+        <v>820</v>
+      </c>
+      <c r="N159">
+        <v>1</v>
+      </c>
+      <c r="O159" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="160" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>822</v>
+      </c>
+      <c r="B160" t="s">
+        <v>823</v>
+      </c>
+      <c r="C160">
+        <v>224.2</v>
+      </c>
+      <c r="D160">
+        <v>257.39999999999998</v>
+      </c>
+      <c r="E160">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="F160" t="s">
+        <v>26</v>
+      </c>
+      <c r="G160" t="s">
+        <v>18</v>
+      </c>
+      <c r="H160" t="s">
+        <v>27</v>
+      </c>
+      <c r="I160" t="s">
+        <v>132</v>
+      </c>
+      <c r="J160" t="s">
+        <v>70</v>
+      </c>
+      <c r="K160" t="s">
+        <v>824</v>
+      </c>
+      <c r="L160">
+        <v>1</v>
+      </c>
+      <c r="M160" t="s">
+        <v>825</v>
+      </c>
+      <c r="N160">
+        <v>1</v>
+      </c>
+      <c r="O160" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="161" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>827</v>
+      </c>
+      <c r="B161" t="s">
+        <v>828</v>
+      </c>
+      <c r="C161">
+        <v>237</v>
+      </c>
+      <c r="D161">
+        <v>270.10000000000002</v>
+      </c>
+      <c r="E161">
+        <v>52</v>
+      </c>
+      <c r="F161" t="s">
+        <v>26</v>
+      </c>
+      <c r="G161" t="s">
+        <v>18</v>
+      </c>
+      <c r="H161" t="s">
+        <v>27</v>
+      </c>
+      <c r="I161" t="s">
+        <v>132</v>
+      </c>
+      <c r="J161" t="s">
+        <v>70</v>
+      </c>
+      <c r="K161" t="s">
+        <v>829</v>
+      </c>
+      <c r="L161">
+        <v>1</v>
+      </c>
+      <c r="M161" t="s">
+        <v>830</v>
+      </c>
+      <c r="N161">
+        <v>1</v>
+      </c>
+      <c r="O161" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>832</v>
+      </c>
+      <c r="B162" t="s">
+        <v>833</v>
+      </c>
+      <c r="C162">
+        <v>249.7</v>
+      </c>
+      <c r="D162">
+        <v>282.7</v>
+      </c>
+      <c r="E162">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="F162" t="s">
+        <v>26</v>
+      </c>
+      <c r="G162" t="s">
+        <v>18</v>
+      </c>
+      <c r="H162" t="s">
+        <v>27</v>
+      </c>
+      <c r="I162" t="s">
+        <v>132</v>
+      </c>
+      <c r="J162" t="s">
+        <v>70</v>
+      </c>
+      <c r="K162" t="s">
+        <v>834</v>
+      </c>
+      <c r="L162">
+        <v>1</v>
+      </c>
+      <c r="M162" t="s">
+        <v>835</v>
+      </c>
+      <c r="N162">
+        <v>1</v>
+      </c>
+      <c r="O162" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>837</v>
+      </c>
+      <c r="B163" t="s">
+        <v>838</v>
+      </c>
+      <c r="C163">
+        <v>262.5</v>
+      </c>
+      <c r="D163">
+        <v>295.3</v>
+      </c>
+      <c r="E163">
+        <v>77.3</v>
+      </c>
+      <c r="F163" t="s">
+        <v>26</v>
+      </c>
+      <c r="G163" t="s">
+        <v>18</v>
+      </c>
+      <c r="H163" t="s">
+        <v>27</v>
+      </c>
+      <c r="I163" t="s">
+        <v>132</v>
+      </c>
+      <c r="J163" t="s">
+        <v>70</v>
+      </c>
+      <c r="K163" t="s">
+        <v>839</v>
+      </c>
+      <c r="L163">
+        <v>1</v>
+      </c>
+      <c r="M163" t="s">
+        <v>840</v>
+      </c>
+      <c r="N163">
+        <v>1</v>
+      </c>
+      <c r="O163" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>842</v>
+      </c>
+      <c r="B164" t="s">
+        <v>843</v>
+      </c>
+      <c r="C164">
+        <v>277</v>
+      </c>
+      <c r="D164">
+        <v>309.8</v>
+      </c>
+      <c r="E164">
+        <v>91.7</v>
+      </c>
+      <c r="F164" t="s">
+        <v>26</v>
+      </c>
+      <c r="G164" t="s">
+        <v>18</v>
+      </c>
+      <c r="H164" t="s">
+        <v>27</v>
+      </c>
+      <c r="I164" t="s">
+        <v>132</v>
+      </c>
+      <c r="J164" t="s">
+        <v>70</v>
+      </c>
+      <c r="K164" t="s">
+        <v>844</v>
+      </c>
+      <c r="L164">
+        <v>1</v>
+      </c>
+      <c r="M164" t="s">
+        <v>845</v>
+      </c>
+      <c r="N164">
+        <v>1</v>
+      </c>
+      <c r="O164" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="165" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>847</v>
+      </c>
+      <c r="B165" t="s">
+        <v>848</v>
+      </c>
+      <c r="C165">
+        <v>289.8</v>
+      </c>
+      <c r="D165">
+        <v>322.5</v>
+      </c>
+      <c r="E165">
+        <v>104.4</v>
+      </c>
+      <c r="F165" t="s">
+        <v>26</v>
+      </c>
+      <c r="G165" t="s">
+        <v>18</v>
+      </c>
+      <c r="H165" t="s">
+        <v>27</v>
+      </c>
+      <c r="I165" t="s">
+        <v>132</v>
+      </c>
+      <c r="J165" t="s">
+        <v>70</v>
+      </c>
+      <c r="K165" t="s">
+        <v>849</v>
+      </c>
+      <c r="L165">
+        <v>1</v>
+      </c>
+      <c r="M165" t="s">
+        <v>850</v>
+      </c>
+      <c r="N165">
+        <v>1</v>
+      </c>
+      <c r="O165" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>852</v>
+      </c>
+      <c r="B166" t="s">
+        <v>853</v>
+      </c>
+      <c r="C166">
+        <v>302.60000000000002</v>
+      </c>
+      <c r="D166">
+        <v>335.1</v>
+      </c>
+      <c r="E166">
+        <v>117</v>
+      </c>
+      <c r="F166" t="s">
+        <v>26</v>
+      </c>
+      <c r="G166" t="s">
+        <v>18</v>
+      </c>
+      <c r="H166" t="s">
+        <v>27</v>
+      </c>
+      <c r="I166" t="s">
+        <v>132</v>
+      </c>
+      <c r="J166" t="s">
+        <v>70</v>
+      </c>
+      <c r="K166" t="s">
+        <v>854</v>
+      </c>
+      <c r="L166">
+        <v>1</v>
+      </c>
+      <c r="M166" t="s">
+        <v>855</v>
+      </c>
+      <c r="N166">
+        <v>1</v>
+      </c>
+      <c r="O166" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="167" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>857</v>
+      </c>
+      <c r="B167" t="s">
+        <v>858</v>
+      </c>
+      <c r="C167">
+        <v>315.3</v>
+      </c>
+      <c r="D167">
+        <v>347.8</v>
+      </c>
+      <c r="E167">
+        <v>129.69999999999999</v>
+      </c>
+      <c r="F167" t="s">
+        <v>26</v>
+      </c>
+      <c r="G167" t="s">
+        <v>18</v>
+      </c>
+      <c r="H167" t="s">
+        <v>27</v>
+      </c>
+      <c r="I167" t="s">
+        <v>132</v>
+      </c>
+      <c r="J167" t="s">
+        <v>70</v>
+      </c>
+      <c r="K167" t="s">
+        <v>859</v>
+      </c>
+      <c r="L167">
+        <v>1</v>
+      </c>
+      <c r="M167" t="s">
+        <v>860</v>
+      </c>
+      <c r="N167">
+        <v>1</v>
+      </c>
+      <c r="O167" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>862</v>
+      </c>
+      <c r="B168" t="s">
+        <v>863</v>
+      </c>
+      <c r="C168">
+        <v>328.1</v>
+      </c>
+      <c r="D168">
+        <v>0.4</v>
+      </c>
+      <c r="E168">
+        <v>142.30000000000001</v>
+      </c>
+      <c r="F168" t="s">
+        <v>26</v>
+      </c>
+      <c r="G168" t="s">
+        <v>18</v>
+      </c>
+      <c r="H168" t="s">
+        <v>27</v>
+      </c>
+      <c r="I168" t="s">
+        <v>132</v>
+      </c>
+      <c r="J168" t="s">
+        <v>70</v>
+      </c>
+      <c r="K168" t="s">
+        <v>864</v>
+      </c>
+      <c r="L168">
+        <v>1</v>
+      </c>
+      <c r="M168" t="s">
+        <v>865</v>
+      </c>
+      <c r="N168">
+        <v>1</v>
+      </c>
+      <c r="O168" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>867</v>
+      </c>
+      <c r="B169" t="s">
+        <v>868</v>
+      </c>
+      <c r="C169">
+        <v>340.9</v>
+      </c>
+      <c r="D169">
+        <v>13.1</v>
+      </c>
+      <c r="E169">
+        <v>155</v>
+      </c>
+      <c r="F169" t="s">
+        <v>26</v>
+      </c>
+      <c r="G169" t="s">
+        <v>18</v>
+      </c>
+      <c r="H169" t="s">
+        <v>27</v>
+      </c>
+      <c r="I169" t="s">
+        <v>132</v>
+      </c>
+      <c r="J169" t="s">
+        <v>70</v>
+      </c>
+      <c r="K169" t="s">
+        <v>869</v>
+      </c>
+      <c r="L169">
+        <v>1</v>
+      </c>
+      <c r="M169" t="s">
+        <v>870</v>
+      </c>
+      <c r="N169">
+        <v>1</v>
+      </c>
+      <c r="O169" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>871</v>
+      </c>
+      <c r="B170" t="s">
+        <v>872</v>
+      </c>
+      <c r="C170">
+        <v>260</v>
+      </c>
+      <c r="D170">
+        <v>271.10000000000002</v>
+      </c>
+      <c r="E170">
+        <v>53.7</v>
+      </c>
+      <c r="F170" t="s">
+        <v>26</v>
+      </c>
+      <c r="G170" t="s">
+        <v>18</v>
+      </c>
+      <c r="H170" t="s">
+        <v>27</v>
+      </c>
+      <c r="I170" t="s">
+        <v>132</v>
+      </c>
+      <c r="J170" t="s">
+        <v>70</v>
+      </c>
+      <c r="K170" t="s">
+        <v>873</v>
+      </c>
+      <c r="L170">
+        <v>1</v>
+      </c>
+      <c r="M170" t="s">
+        <v>874</v>
+      </c>
+      <c r="N170">
+        <v>1</v>
+      </c>
+      <c r="O170" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="171" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>876</v>
+      </c>
+      <c r="B171" t="s">
+        <v>877</v>
+      </c>
+      <c r="C171">
+        <v>272.8</v>
+      </c>
+      <c r="D171">
+        <v>283.7</v>
+      </c>
+      <c r="E171">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="F171" t="s">
+        <v>26</v>
+      </c>
+      <c r="G171" t="s">
+        <v>18</v>
+      </c>
+      <c r="H171" t="s">
+        <v>27</v>
+      </c>
+      <c r="I171" t="s">
+        <v>132</v>
+      </c>
+      <c r="J171" t="s">
+        <v>70</v>
+      </c>
+      <c r="K171" t="s">
+        <v>878</v>
+      </c>
+      <c r="L171">
+        <v>1</v>
+      </c>
+      <c r="M171" t="s">
+        <v>879</v>
+      </c>
+      <c r="N171">
+        <v>1</v>
+      </c>
+      <c r="O171" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>881</v>
+      </c>
+      <c r="B172" t="s">
+        <v>882</v>
+      </c>
+      <c r="C172">
+        <v>285.5</v>
+      </c>
+      <c r="D172">
+        <v>296.3</v>
+      </c>
+      <c r="E172">
+        <v>79</v>
+      </c>
+      <c r="F172" t="s">
+        <v>26</v>
+      </c>
+      <c r="G172" t="s">
+        <v>18</v>
+      </c>
+      <c r="H172" t="s">
+        <v>27</v>
+      </c>
+      <c r="I172" t="s">
+        <v>132</v>
+      </c>
+      <c r="J172" t="s">
+        <v>70</v>
+      </c>
+      <c r="K172" t="s">
+        <v>883</v>
+      </c>
+      <c r="L172">
+        <v>1</v>
+      </c>
+      <c r="M172" t="s">
+        <v>884</v>
+      </c>
+      <c r="N172">
+        <v>1</v>
+      </c>
+      <c r="O172" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="173" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>886</v>
+      </c>
+      <c r="B173" t="s">
+        <v>887</v>
+      </c>
+      <c r="C173">
+        <v>299.2</v>
+      </c>
+      <c r="D173">
+        <v>309.89999999999998</v>
+      </c>
+      <c r="E173">
+        <v>92.6</v>
+      </c>
+      <c r="F173" t="s">
+        <v>26</v>
+      </c>
+      <c r="G173" t="s">
+        <v>18</v>
+      </c>
+      <c r="H173" t="s">
+        <v>27</v>
+      </c>
+      <c r="I173" t="s">
+        <v>132</v>
+      </c>
+      <c r="J173" t="s">
+        <v>70</v>
+      </c>
+      <c r="K173" t="s">
+        <v>888</v>
+      </c>
+      <c r="L173">
+        <v>1</v>
+      </c>
+      <c r="M173" t="s">
+        <v>889</v>
+      </c>
+      <c r="N173">
+        <v>1</v>
+      </c>
+      <c r="O173" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>891</v>
+      </c>
+      <c r="B174" t="s">
+        <v>892</v>
+      </c>
+      <c r="C174">
+        <v>311.89999999999998</v>
+      </c>
+      <c r="D174">
+        <v>322.5</v>
+      </c>
+      <c r="E174">
+        <v>105.2</v>
+      </c>
+      <c r="F174" t="s">
+        <v>26</v>
+      </c>
+      <c r="G174" t="s">
+        <v>18</v>
+      </c>
+      <c r="H174" t="s">
+        <v>27</v>
+      </c>
+      <c r="I174" t="s">
+        <v>132</v>
+      </c>
+      <c r="J174" t="s">
+        <v>70</v>
+      </c>
+      <c r="K174" t="s">
+        <v>893</v>
+      </c>
+      <c r="L174">
+        <v>1</v>
+      </c>
+      <c r="M174" t="s">
+        <v>894</v>
+      </c>
+      <c r="N174">
+        <v>1</v>
+      </c>
+      <c r="O174" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>896</v>
+      </c>
+      <c r="B175" t="s">
+        <v>897</v>
+      </c>
+      <c r="C175">
+        <v>324.7</v>
+      </c>
+      <c r="D175">
+        <v>335.1</v>
+      </c>
+      <c r="E175">
+        <v>117.8</v>
+      </c>
+      <c r="F175" t="s">
+        <v>26</v>
+      </c>
+      <c r="G175" t="s">
+        <v>18</v>
+      </c>
+      <c r="H175" t="s">
+        <v>27</v>
+      </c>
+      <c r="I175" t="s">
+        <v>132</v>
+      </c>
+      <c r="J175" t="s">
+        <v>70</v>
+      </c>
+      <c r="K175" t="s">
+        <v>898</v>
+      </c>
+      <c r="L175">
+        <v>1</v>
+      </c>
+      <c r="M175" t="s">
+        <v>899</v>
+      </c>
+      <c r="N175">
+        <v>1</v>
+      </c>
+      <c r="O175" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>901</v>
+      </c>
+      <c r="B176" t="s">
+        <v>902</v>
+      </c>
+      <c r="C176">
+        <v>337.4</v>
+      </c>
+      <c r="D176">
+        <v>347.8</v>
+      </c>
+      <c r="E176">
+        <v>130.5</v>
+      </c>
+      <c r="F176" t="s">
+        <v>26</v>
+      </c>
+      <c r="G176" t="s">
+        <v>18</v>
+      </c>
+      <c r="H176" t="s">
+        <v>27</v>
+      </c>
+      <c r="I176" t="s">
+        <v>132</v>
+      </c>
+      <c r="J176" t="s">
+        <v>70</v>
+      </c>
+      <c r="K176" t="s">
+        <v>903</v>
+      </c>
+      <c r="L176">
+        <v>1</v>
+      </c>
+      <c r="M176" t="s">
+        <v>904</v>
+      </c>
+      <c r="N176">
+        <v>1</v>
+      </c>
+      <c r="O176" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>906</v>
+      </c>
+      <c r="B177" t="s">
+        <v>907</v>
+      </c>
+      <c r="C177">
+        <v>350.2</v>
+      </c>
+      <c r="D177">
+        <v>0.4</v>
+      </c>
+      <c r="E177">
+        <v>143.1</v>
+      </c>
+      <c r="F177" t="s">
+        <v>26</v>
+      </c>
+      <c r="G177" t="s">
+        <v>18</v>
+      </c>
+      <c r="H177" t="s">
+        <v>27</v>
+      </c>
+      <c r="I177" t="s">
+        <v>132</v>
+      </c>
+      <c r="J177" t="s">
+        <v>70</v>
+      </c>
+      <c r="K177" t="s">
+        <v>908</v>
+      </c>
+      <c r="L177">
+        <v>1</v>
+      </c>
+      <c r="M177" t="s">
+        <v>909</v>
+      </c>
+      <c r="N177">
+        <v>1</v>
+      </c>
+      <c r="O177" t="s">
+        <v>910</v>
       </c>
     </row>
   </sheetData>
@@ -9192,8 +11943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F58391A-1A18-48BB-B42D-F47ACF826E68}">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
@@ -10053,39 +12804,39 @@
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A130">
+      <c r="A130" t="str">
         <f>'Catalog-static'!A130</f>
-        <v>0</v>
+        <v>20241023UTa</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A131">
+      <c r="A131" t="str">
         <f>'Catalog-static'!A131</f>
-        <v>0</v>
+        <v>20241027UTa</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A132">
+      <c r="A132" t="str">
         <f>'Catalog-static'!A132</f>
-        <v>0</v>
+        <v>20241027UTb</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A133">
+      <c r="A133" t="str">
         <f>'Catalog-static'!A133</f>
-        <v>0</v>
+        <v>20241027UTc</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A134">
+      <c r="A134" t="str">
         <f>'Catalog-static'!A134</f>
-        <v>0</v>
+        <v>20241027UTd</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A135">
+      <c r="A135" t="str">
         <f>'Catalog-static'!A135</f>
-        <v>0</v>
+        <v>20241027UTe</v>
       </c>
     </row>
   </sheetData>
@@ -10098,14 +12849,14 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="5.54296875" style="21" customWidth="1"/>
     <col min="7" max="7" width="11.1796875" style="21" customWidth="1"/>
     <col min="8" max="8" width="12.453125" customWidth="1"/>
   </cols>
@@ -12082,4 +14833,642 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FB822E-4FB0-4362-8846-871BD8F7A1EF}">
+  <dimension ref="A1:E48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="47.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
+        <v>685</v>
+      </c>
+      <c r="B1" s="18">
+        <f>SUM(B2:B99)</f>
+        <v>349</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>698</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>688</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="32">
+        <v>45554</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>689</v>
+      </c>
+      <c r="D2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="32">
+        <v>45558</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>689</v>
+      </c>
+      <c r="D3" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="32">
+        <v>45560</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>689</v>
+      </c>
+      <c r="D4" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="32">
+        <v>45564</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>689</v>
+      </c>
+      <c r="D5" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="32">
+        <v>45567</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>689</v>
+      </c>
+      <c r="D6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="32">
+        <v>45571</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>689</v>
+      </c>
+      <c r="D7" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="32">
+        <v>45572</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>689</v>
+      </c>
+      <c r="D8" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="32">
+        <v>45573</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>689</v>
+      </c>
+      <c r="D9" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="32">
+        <v>45574</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>689</v>
+      </c>
+      <c r="D10" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="32">
+        <v>45575</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>689</v>
+      </c>
+      <c r="D11" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="32">
+        <v>45579</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>689</v>
+      </c>
+      <c r="D12" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="32">
+        <v>45581</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>689</v>
+      </c>
+      <c r="D13" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="32">
+        <v>45587</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>689</v>
+      </c>
+      <c r="D14" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="32">
+        <v>45588</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>689</v>
+      </c>
+      <c r="D15" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="32">
+        <v>45592</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>689</v>
+      </c>
+      <c r="D16" t="s">
+        <v>697</v>
+      </c>
+      <c r="E16" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="32">
+        <v>45601</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>689</v>
+      </c>
+      <c r="D17" t="s">
+        <v>697</v>
+      </c>
+      <c r="E17" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="32">
+        <v>45607</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>689</v>
+      </c>
+      <c r="D18" t="s">
+        <v>914</v>
+      </c>
+      <c r="E18" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="32">
+        <v>45611</v>
+      </c>
+      <c r="B19">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>689</v>
+      </c>
+      <c r="D19" t="s">
+        <v>697</v>
+      </c>
+      <c r="E19" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="32">
+        <v>45614</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>689</v>
+      </c>
+      <c r="D20" t="s">
+        <v>697</v>
+      </c>
+      <c r="E20" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="32">
+        <v>45617</v>
+      </c>
+      <c r="B21">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>689</v>
+      </c>
+      <c r="D21" t="s">
+        <v>914</v>
+      </c>
+      <c r="E21" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="32">
+        <v>45620</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>689</v>
+      </c>
+      <c r="D22" t="s">
+        <v>914</v>
+      </c>
+      <c r="E22" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="32">
+        <v>45624</v>
+      </c>
+      <c r="B23">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>689</v>
+      </c>
+      <c r="D23" t="s">
+        <v>914</v>
+      </c>
+      <c r="E23" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="32">
+        <v>45625</v>
+      </c>
+      <c r="B24">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>689</v>
+      </c>
+      <c r="D24" t="s">
+        <v>697</v>
+      </c>
+      <c r="E24" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="32">
+        <v>45628</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>689</v>
+      </c>
+      <c r="D25" t="s">
+        <v>697</v>
+      </c>
+      <c r="E25" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="32">
+        <v>45629</v>
+      </c>
+      <c r="B26">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>689</v>
+      </c>
+      <c r="D26" t="s">
+        <v>697</v>
+      </c>
+      <c r="E26" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="32">
+        <v>45631</v>
+      </c>
+      <c r="B27">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>689</v>
+      </c>
+      <c r="D27" t="s">
+        <v>697</v>
+      </c>
+      <c r="E27" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="32">
+        <v>45657</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="32">
+        <v>45663</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="32">
+        <v>45671</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="32">
+        <v>45672</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="E31" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="32">
+        <v>45673</v>
+      </c>
+      <c r="B32">
+        <v>23</v>
+      </c>
+      <c r="E32" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="32">
+        <v>45674</v>
+      </c>
+      <c r="B33">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>689</v>
+      </c>
+      <c r="E33" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="32">
+        <v>45684</v>
+      </c>
+      <c r="B34">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>926</v>
+      </c>
+      <c r="E34" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="32">
+        <v>45685</v>
+      </c>
+      <c r="B35">
+        <v>19</v>
+      </c>
+      <c r="C35" t="s">
+        <v>913</v>
+      </c>
+      <c r="E35" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="32">
+        <v>45686</v>
+      </c>
+      <c r="B36">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>689</v>
+      </c>
+      <c r="D36" t="s">
+        <v>697</v>
+      </c>
+      <c r="E36" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="32">
+        <v>45688</v>
+      </c>
+      <c r="B37">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="32">
+        <v>45695</v>
+      </c>
+      <c r="B38">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="32"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="32"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="32"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="32"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="32"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="32"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="32"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="32"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="32"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E43EC747-111A-4BB5-BFE1-00E73C62C53D}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>690</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>694</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to ROIs for SED and EZ Disturbance - AGU abstract
Made additions to the ROI code to include the 2024-25 SED disturbance and fixed a problem with the variance map plots.

**Still need to have a uniform approach to limb correction, contiguous map overlap longitude range, and add Pat's pressure dependent ammonia correction.
</commit_message>
<xml_diff>
--- a/Catalog/Catalog-static.xlsx
+++ b/Catalog/Catalog-static.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96837D24-0DF5-43F6-B6D7-617BA7B9FD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66B011A-2394-4154-9032-218BDB7E609E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Catalog-static'!$A$1:$O$102</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26081,7 +26082,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Profiles updates and new observations
Updated the profiles code to run with 2025-26 data. Completed processing of 2025-26 data through 2025-09-30.
</commit_message>
<xml_diff>
--- a/Catalog/Catalog-static.xlsx
+++ b/Catalog/Catalog-static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66B011A-2394-4154-9032-218BDB7E609E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE072B2A-28D5-45FC-BB6E-5ECFC660D330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalog-static" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Catalog-static'!$A$1:$O$102</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3893" uniqueCount="1831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3906" uniqueCount="1833">
   <si>
     <t>ObsID</t>
   </si>
@@ -5570,6 +5569,12 @@
   </si>
   <si>
     <t>Flats taken! Poor to fair focus, Good GRS, Good SEB outbreak; Quality is pretty variable</t>
+  </si>
+  <si>
+    <t>Tenth was not userful due to twilight</t>
+  </si>
+  <si>
+    <t>Eighth is not useful due to twilight</t>
   </si>
 </sst>
 </file>
@@ -26082,8 +26087,8 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26100,7 +26105,7 @@
       </c>
       <c r="B1" s="18">
         <f>SUM(B2:B99)</f>
-        <v>383</v>
+        <v>421</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>696</v>
@@ -26553,8 +26558,11 @@
       <c r="B30">
         <v>8</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>910</v>
+      <c r="C30" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="D30" t="s">
+        <v>695</v>
       </c>
       <c r="E30" t="s">
         <v>1556</v>
@@ -26736,8 +26744,11 @@
       <c r="B42">
         <v>7</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="35" t="s">
         <v>910</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1828</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -26758,19 +26769,77 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="32"/>
+      <c r="A44" s="32">
+        <v>45919</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>687</v>
+      </c>
+      <c r="D44" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="32"/>
+      <c r="A45" s="32">
+        <v>45925</v>
+      </c>
+      <c r="B45">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>687</v>
+      </c>
+      <c r="D45" t="s">
+        <v>695</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1832</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="32"/>
+      <c r="A46" s="32">
+        <v>45926</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>687</v>
+      </c>
+      <c r="D46" t="s">
+        <v>695</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1832</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="32"/>
+      <c r="A47" s="32">
+        <v>45930</v>
+      </c>
+      <c r="B47">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>910</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1831</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="32"/>
+      <c r="A48" s="32">
+        <v>45931</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1831</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Precursor commit to major update of MakeContiguousMap
Some new processed data and some smallish updates to code
</commit_message>
<xml_diff>
--- a/Catalog/Catalog-static.xlsx
+++ b/Catalog/Catalog-static.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE072B2A-28D5-45FC-BB6E-5ECFC660D330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD7AEAE-997A-467A-A37A-24B9C24FB288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="990" windowWidth="19190" windowHeight="9810" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalog-static" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3906" uniqueCount="1833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4350" uniqueCount="2049">
   <si>
     <t>ObsID</t>
   </si>
@@ -5574,7 +5574,655 @@
     <t>Tenth was not userful due to twilight</t>
   </si>
   <si>
-    <t>Eighth is not useful due to twilight</t>
+    <t>Eighth is not useful due to twilight - moon/shadow?</t>
+  </si>
+  <si>
+    <t>20250919UTa</t>
+  </si>
+  <si>
+    <t>2025-09-19_10:27:06</t>
+  </si>
+  <si>
+    <t>2025-09-19-1027_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1027_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1037_7-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250919UTb</t>
+  </si>
+  <si>
+    <t>2025-09-19_10:48:12</t>
+  </si>
+  <si>
+    <t>2025-09-19-1048_2-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1048_2-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1058_8-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250919UTc</t>
+  </si>
+  <si>
+    <t>2025-09-19_11:09:24</t>
+  </si>
+  <si>
+    <t>2025-09-19-1109_4-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1109_4-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1120_0-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250919UTd</t>
+  </si>
+  <si>
+    <t>2025-09-19_11:30:36</t>
+  </si>
+  <si>
+    <t>2025-09-19-1130_6-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1130_6-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1141_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250919UTe</t>
+  </si>
+  <si>
+    <t>2025-09-19_11:51:42</t>
+  </si>
+  <si>
+    <t>2025-09-19-1151_7-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1151_7-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1202_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250919UTf</t>
+  </si>
+  <si>
+    <t>2025-09-19_12:12:54</t>
+  </si>
+  <si>
+    <t>2025-09-19-1212_9-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-19-1212_9-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>20250925UTa</t>
+  </si>
+  <si>
+    <t>2025-09-25_10:04:42</t>
+  </si>
+  <si>
+    <t>2025-09-25-1004_7-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1004_7-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1015_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250925UTb</t>
+  </si>
+  <si>
+    <t>2025-09-25_10:29:06</t>
+  </si>
+  <si>
+    <t>2025-09-25-1029_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1029_1-Jupiter_R656G647B632-RGB-WhtBal-647shift</t>
+  </si>
+  <si>
+    <t>2025-09-25-1039_7-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250925UTc</t>
+  </si>
+  <si>
+    <t>2025-09-25_10:50:18</t>
+  </si>
+  <si>
+    <t>2025-09-25-1050_3-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1050_3-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1100_9-Jupiter_R685G550B450-RGB_ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250925UTd</t>
+  </si>
+  <si>
+    <t>2025-09-25_11:11:30</t>
+  </si>
+  <si>
+    <t>2025-09-25-1111_4-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1111_5-Jupiter_R656G647B632-RGB-WhtBal-647shift</t>
+  </si>
+  <si>
+    <t>2025-09-25-1122_0-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250925UTe</t>
+  </si>
+  <si>
+    <t>2025-09-25_11:32:36</t>
+  </si>
+  <si>
+    <t>2025-09-25-1132_6-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1132_6-Jupiter_R656G647B632-RGB-WhtBal-shift</t>
+  </si>
+  <si>
+    <t>2025-09-25-1143_2-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250925UTf</t>
+  </si>
+  <si>
+    <t>2025-09-25_11:53:48</t>
+  </si>
+  <si>
+    <t>2025-09-25-1153_8-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1153_8-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1204_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250925UTg</t>
+  </si>
+  <si>
+    <t>2025-09-25_12:15:36</t>
+  </si>
+  <si>
+    <t>2025-09-25-1214_9-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1215_6-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1225_5-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250925UTh</t>
+  </si>
+  <si>
+    <t>2025-09-25_12:36:06</t>
+  </si>
+  <si>
+    <t>2025-09-25-1236_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1236_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-25-1246_7-Jupiter_R685G550B450-RGB-ClrSmth_WhtBal-Shift-WV</t>
+  </si>
+  <si>
+    <t>20250926UTa</t>
+  </si>
+  <si>
+    <t>2025-09-26_10:06:42</t>
+  </si>
+  <si>
+    <t>2025-09-26-1006_7-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1006_7-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1017_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250926UTb</t>
+  </si>
+  <si>
+    <t>2025-09-26_10:27:54</t>
+  </si>
+  <si>
+    <t>2025-09-26-1027_9-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1027_9-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1038_5-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250926UTc</t>
+  </si>
+  <si>
+    <t>2025-09-26_10:49:00</t>
+  </si>
+  <si>
+    <t>2025-09-26-1049_0-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1049_0-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1059_6-Jupiter_R685G550B450-RGB-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250926UTd</t>
+  </si>
+  <si>
+    <t>2025-09-26_11:10:12</t>
+  </si>
+  <si>
+    <t>2025-09-26-1110_2-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1110_2-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1120_8-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250926UTe</t>
+  </si>
+  <si>
+    <t>2025-09-26_11:31:24</t>
+  </si>
+  <si>
+    <t>2025-09-26-1131_4-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1131_4-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1142_0-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250926UTf</t>
+  </si>
+  <si>
+    <t>2025-09-26_11:52:30</t>
+  </si>
+  <si>
+    <t>2025-09-26-1152_5-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1152_5-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1203_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250926UTg</t>
+  </si>
+  <si>
+    <t>2025-09-26_12:13:42</t>
+  </si>
+  <si>
+    <t>2025-09-26-1213_7-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1213_7-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1224_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250926UTh</t>
+  </si>
+  <si>
+    <t>2025-09-26_12:34:48</t>
+  </si>
+  <si>
+    <t>2025-09-26-1234_8-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1234_8-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-26-1245_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250930UTa</t>
+  </si>
+  <si>
+    <t>2025-09-30_09:15:42</t>
+  </si>
+  <si>
+    <t>2025-09-30-0915_7-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-0915_7-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-0926_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250930UTb</t>
+  </si>
+  <si>
+    <t>2025-09-30_09:36:48</t>
+  </si>
+  <si>
+    <t>2025-09-30-0936_8-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-0936_8-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-0947_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250930UTc</t>
+  </si>
+  <si>
+    <t>2025-09-30_09:58:00</t>
+  </si>
+  <si>
+    <t>2025-09-30-0958_0-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1008_6-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250930UTd</t>
+  </si>
+  <si>
+    <t>2025-09-30_10:19:06</t>
+  </si>
+  <si>
+    <t>2025-09-30-1019_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1019_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1029_7-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250930UTe</t>
+  </si>
+  <si>
+    <t>2025-09-30_10:40:18</t>
+  </si>
+  <si>
+    <t>2025-09-30-1040_3-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1040_3-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1050_9-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250930UTf</t>
+  </si>
+  <si>
+    <t>2025-09-30_11:01:30</t>
+  </si>
+  <si>
+    <t>2025-09-30-1101_5-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1101_5-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1112_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250930UTg</t>
+  </si>
+  <si>
+    <t>2025-09-30_11:22:36</t>
+  </si>
+  <si>
+    <t>2025-09-30-1122_6-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1122_6-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1133_2-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250930UTh</t>
+  </si>
+  <si>
+    <t>2025-09-30_11:43:48</t>
+  </si>
+  <si>
+    <t>2025-09-30-1143_8-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1143_8-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1154_4-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250930UTi</t>
+  </si>
+  <si>
+    <t>2025-09-30_12:04:54</t>
+  </si>
+  <si>
+    <t>2025-09-30-1205_0-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1204_9-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1215_5-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20250930UTj</t>
+  </si>
+  <si>
+    <t>2025-09-30_12:26:06</t>
+  </si>
+  <si>
+    <t>2025-09-30-1226_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1226_1-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-09-30-1236_7-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTa</t>
+  </si>
+  <si>
+    <t>2025-10-01_09:16:24</t>
+  </si>
+  <si>
+    <t>2025-10-01-0916_4-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-0916_4-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-0927_0-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTb</t>
+  </si>
+  <si>
+    <t>2025-10-01_09:37:36</t>
+  </si>
+  <si>
+    <t>2025-10-01-0937_6-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-0937_6-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-0948_2-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTc</t>
+  </si>
+  <si>
+    <t>2025-10-01_09:58:48</t>
+  </si>
+  <si>
+    <t>2025-10-01-0958_7-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-0958_8-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1009_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTd</t>
+  </si>
+  <si>
+    <t>2025-10-01_10:19:54</t>
+  </si>
+  <si>
+    <t>2025-10-01-1019_9-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1019_9-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1030_5-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTe</t>
+  </si>
+  <si>
+    <t>2025-10-01_10:40:48</t>
+  </si>
+  <si>
+    <t>2025-10-01-1041_1-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1040_8-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1051_7-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTf</t>
+  </si>
+  <si>
+    <t>2025-10-01_11:02:12</t>
+  </si>
+  <si>
+    <t>2025-10-01-1102_2-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1102_2-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1112_8-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTg</t>
+  </si>
+  <si>
+    <t>2025-10-01_11:23:24</t>
+  </si>
+  <si>
+    <t>2025-10-01-1123_4-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1123_4-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1134_0-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTh</t>
+  </si>
+  <si>
+    <t>2025-10-01_11:44:30</t>
+  </si>
+  <si>
+    <t>2025-10-01-1144_5-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1144_5-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1155_1-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTi</t>
+  </si>
+  <si>
+    <t>2025-10-01_12:05:42</t>
+  </si>
+  <si>
+    <t>2025-10-01-1205_7-Jupiter_R656G620B632-RGB-WhtBal-Shift656-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1205_7-Jupiter_R656G647B632-RGB-Shift647+632-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1216_3-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTj</t>
+  </si>
+  <si>
+    <t>2025-10-01_12:26:54</t>
+  </si>
+  <si>
+    <t>2025-10-01-1226_9-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1226_9-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1237_5-Jupiter_R685G550B450-RGB-ClrSmth-WhtBal-WV</t>
+  </si>
+  <si>
+    <t>20251001UTk</t>
+  </si>
+  <si>
+    <t>2025-10-01_12:48:00</t>
+  </si>
+  <si>
+    <t>2025-10-01-1248_0-Jupiter_R656G620B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>2025-10-01-1248_0-Jupiter_R656G647B632-RGB-WhtBal</t>
+  </si>
+  <si>
+    <t>Heavy dew forced an early end due to reduce SNR</t>
+  </si>
+  <si>
+    <t>First five are blurry, then refocued. Last RGB is missing G&amp;B due to meridian+10 crossing</t>
+  </si>
+  <si>
+    <t>Cloudy early in the morning, then cleared around 3:30</t>
+  </si>
+  <si>
+    <t>First night with shorter (60s v 90s) IrGB videos; very poor seeing; The 1103UT 632OI video is too dim to stack</t>
   </si>
 </sst>
 </file>
@@ -6571,13 +7219,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O357"/>
+  <dimension ref="A1:O400"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B349" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B385" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B352" sqref="B352"/>
+      <selection pane="bottomRight" activeCell="C393" sqref="C393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23178,6 +23826,2027 @@
       </c>
       <c r="O357" t="s">
         <v>1827</v>
+      </c>
+    </row>
+    <row r="358" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A358" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B358" t="s">
+        <v>1834</v>
+      </c>
+      <c r="C358">
+        <v>6.1</v>
+      </c>
+      <c r="D358">
+        <v>314.39999999999998</v>
+      </c>
+      <c r="E358">
+        <v>174.6</v>
+      </c>
+      <c r="F358" t="s">
+        <v>26</v>
+      </c>
+      <c r="G358" t="s">
+        <v>18</v>
+      </c>
+      <c r="H358" t="s">
+        <v>27</v>
+      </c>
+      <c r="I358" t="s">
+        <v>132</v>
+      </c>
+      <c r="J358" t="s">
+        <v>70</v>
+      </c>
+      <c r="K358" t="s">
+        <v>1835</v>
+      </c>
+      <c r="L358">
+        <v>1</v>
+      </c>
+      <c r="M358" t="s">
+        <v>1836</v>
+      </c>
+      <c r="N358">
+        <v>1</v>
+      </c>
+      <c r="O358" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="359" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A359" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B359" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C359">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="D359">
+        <v>327.2</v>
+      </c>
+      <c r="E359">
+        <v>187.3</v>
+      </c>
+      <c r="F359" t="s">
+        <v>26</v>
+      </c>
+      <c r="G359" t="s">
+        <v>18</v>
+      </c>
+      <c r="H359" t="s">
+        <v>27</v>
+      </c>
+      <c r="I359" t="s">
+        <v>132</v>
+      </c>
+      <c r="J359" t="s">
+        <v>70</v>
+      </c>
+      <c r="K359" t="s">
+        <v>1840</v>
+      </c>
+      <c r="L359">
+        <v>1</v>
+      </c>
+      <c r="M359" t="s">
+        <v>1841</v>
+      </c>
+      <c r="N359">
+        <v>1</v>
+      </c>
+      <c r="O359" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="360" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A360" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B360" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C360">
+        <v>31.9</v>
+      </c>
+      <c r="D360">
+        <v>340</v>
+      </c>
+      <c r="E360">
+        <v>200.1</v>
+      </c>
+      <c r="F360" t="s">
+        <v>26</v>
+      </c>
+      <c r="G360" t="s">
+        <v>18</v>
+      </c>
+      <c r="H360" t="s">
+        <v>27</v>
+      </c>
+      <c r="I360" t="s">
+        <v>132</v>
+      </c>
+      <c r="J360" t="s">
+        <v>70</v>
+      </c>
+      <c r="K360" t="s">
+        <v>1845</v>
+      </c>
+      <c r="L360">
+        <v>1</v>
+      </c>
+      <c r="M360" t="s">
+        <v>1846</v>
+      </c>
+      <c r="N360">
+        <v>1</v>
+      </c>
+      <c r="O360" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="361" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A361" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B361" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C361">
+        <v>44.8</v>
+      </c>
+      <c r="D361">
+        <v>352.8</v>
+      </c>
+      <c r="E361">
+        <v>213</v>
+      </c>
+      <c r="F361" t="s">
+        <v>26</v>
+      </c>
+      <c r="G361" t="s">
+        <v>18</v>
+      </c>
+      <c r="H361" t="s">
+        <v>27</v>
+      </c>
+      <c r="I361" t="s">
+        <v>132</v>
+      </c>
+      <c r="J361" t="s">
+        <v>70</v>
+      </c>
+      <c r="K361" t="s">
+        <v>1850</v>
+      </c>
+      <c r="L361">
+        <v>1</v>
+      </c>
+      <c r="M361" t="s">
+        <v>1851</v>
+      </c>
+      <c r="N361">
+        <v>1</v>
+      </c>
+      <c r="O361" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="362" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A362" t="s">
+        <v>1853</v>
+      </c>
+      <c r="B362" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C362">
+        <v>57.6</v>
+      </c>
+      <c r="D362">
+        <v>5.5</v>
+      </c>
+      <c r="E362">
+        <v>225.7</v>
+      </c>
+      <c r="F362" t="s">
+        <v>26</v>
+      </c>
+      <c r="G362" t="s">
+        <v>18</v>
+      </c>
+      <c r="H362" t="s">
+        <v>27</v>
+      </c>
+      <c r="I362" t="s">
+        <v>132</v>
+      </c>
+      <c r="J362" t="s">
+        <v>70</v>
+      </c>
+      <c r="K362" t="s">
+        <v>1855</v>
+      </c>
+      <c r="L362">
+        <v>1</v>
+      </c>
+      <c r="M362" t="s">
+        <v>1856</v>
+      </c>
+      <c r="N362">
+        <v>1</v>
+      </c>
+      <c r="O362" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="363" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A363" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B363" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C363">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="D363">
+        <v>18.3</v>
+      </c>
+      <c r="E363">
+        <v>238.5</v>
+      </c>
+      <c r="F363" t="s">
+        <v>26</v>
+      </c>
+      <c r="G363" t="s">
+        <v>18</v>
+      </c>
+      <c r="H363" t="s">
+        <v>27</v>
+      </c>
+      <c r="I363" t="s">
+        <v>132</v>
+      </c>
+      <c r="J363" t="s">
+        <v>70</v>
+      </c>
+      <c r="K363" t="s">
+        <v>1860</v>
+      </c>
+      <c r="L363">
+        <v>1</v>
+      </c>
+      <c r="M363" t="s">
+        <v>1861</v>
+      </c>
+      <c r="N363">
+        <v>1</v>
+      </c>
+      <c r="O363" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="364" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A364" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B364" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C364">
+        <v>219.4</v>
+      </c>
+      <c r="D364">
+        <v>122.1</v>
+      </c>
+      <c r="E364">
+        <v>343.9</v>
+      </c>
+      <c r="F364" t="s">
+        <v>26</v>
+      </c>
+      <c r="G364" t="s">
+        <v>18</v>
+      </c>
+      <c r="H364" t="s">
+        <v>27</v>
+      </c>
+      <c r="I364" t="s">
+        <v>132</v>
+      </c>
+      <c r="J364" t="s">
+        <v>70</v>
+      </c>
+      <c r="K364" t="s">
+        <v>1864</v>
+      </c>
+      <c r="L364">
+        <v>1</v>
+      </c>
+      <c r="M364" t="s">
+        <v>1865</v>
+      </c>
+      <c r="N364">
+        <v>1</v>
+      </c>
+      <c r="O364" t="s">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="365" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A365" t="s">
+        <v>1867</v>
+      </c>
+      <c r="B365" t="s">
+        <v>1868</v>
+      </c>
+      <c r="C365">
+        <v>234.3</v>
+      </c>
+      <c r="D365">
+        <v>136.9</v>
+      </c>
+      <c r="E365">
+        <v>358.6</v>
+      </c>
+      <c r="F365" t="s">
+        <v>26</v>
+      </c>
+      <c r="G365" t="s">
+        <v>18</v>
+      </c>
+      <c r="H365" t="s">
+        <v>27</v>
+      </c>
+      <c r="I365" t="s">
+        <v>132</v>
+      </c>
+      <c r="J365" t="s">
+        <v>70</v>
+      </c>
+      <c r="K365" t="s">
+        <v>1869</v>
+      </c>
+      <c r="L365">
+        <v>1</v>
+      </c>
+      <c r="M365" t="s">
+        <v>1870</v>
+      </c>
+      <c r="N365">
+        <v>1</v>
+      </c>
+      <c r="O365" t="s">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="366" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A366" t="s">
+        <v>1872</v>
+      </c>
+      <c r="B366" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C366">
+        <v>247.2</v>
+      </c>
+      <c r="D366">
+        <v>149.69999999999999</v>
+      </c>
+      <c r="E366">
+        <v>11.4</v>
+      </c>
+      <c r="F366" t="s">
+        <v>26</v>
+      </c>
+      <c r="G366" t="s">
+        <v>18</v>
+      </c>
+      <c r="H366" t="s">
+        <v>27</v>
+      </c>
+      <c r="I366" t="s">
+        <v>132</v>
+      </c>
+      <c r="J366" t="s">
+        <v>70</v>
+      </c>
+      <c r="K366" t="s">
+        <v>1874</v>
+      </c>
+      <c r="L366">
+        <v>1</v>
+      </c>
+      <c r="M366" t="s">
+        <v>1875</v>
+      </c>
+      <c r="N366">
+        <v>1</v>
+      </c>
+      <c r="O366" t="s">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="367" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A367" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B367" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C367">
+        <v>260.2</v>
+      </c>
+      <c r="D367">
+        <v>162.5</v>
+      </c>
+      <c r="E367">
+        <v>24.2</v>
+      </c>
+      <c r="F367" t="s">
+        <v>26</v>
+      </c>
+      <c r="G367" t="s">
+        <v>18</v>
+      </c>
+      <c r="H367" t="s">
+        <v>27</v>
+      </c>
+      <c r="I367" t="s">
+        <v>132</v>
+      </c>
+      <c r="J367" t="s">
+        <v>70</v>
+      </c>
+      <c r="K367" t="s">
+        <v>1879</v>
+      </c>
+      <c r="L367">
+        <v>1</v>
+      </c>
+      <c r="M367" t="s">
+        <v>1880</v>
+      </c>
+      <c r="N367">
+        <v>1</v>
+      </c>
+      <c r="O367" t="s">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="368" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A368" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B368" t="s">
+        <v>1883</v>
+      </c>
+      <c r="C368">
+        <v>273</v>
+      </c>
+      <c r="D368">
+        <v>175.2</v>
+      </c>
+      <c r="E368">
+        <v>37</v>
+      </c>
+      <c r="F368" t="s">
+        <v>26</v>
+      </c>
+      <c r="G368" t="s">
+        <v>18</v>
+      </c>
+      <c r="H368" t="s">
+        <v>27</v>
+      </c>
+      <c r="I368" t="s">
+        <v>132</v>
+      </c>
+      <c r="J368" t="s">
+        <v>70</v>
+      </c>
+      <c r="K368" t="s">
+        <v>1884</v>
+      </c>
+      <c r="L368">
+        <v>1</v>
+      </c>
+      <c r="M368" t="s">
+        <v>1885</v>
+      </c>
+      <c r="N368">
+        <v>1</v>
+      </c>
+      <c r="O368" t="s">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="369" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A369" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B369" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C369">
+        <v>285.89999999999998</v>
+      </c>
+      <c r="D369">
+        <v>188</v>
+      </c>
+      <c r="E369">
+        <v>49.8</v>
+      </c>
+      <c r="F369" t="s">
+        <v>26</v>
+      </c>
+      <c r="G369" t="s">
+        <v>18</v>
+      </c>
+      <c r="H369" t="s">
+        <v>27</v>
+      </c>
+      <c r="I369" t="s">
+        <v>132</v>
+      </c>
+      <c r="J369" t="s">
+        <v>70</v>
+      </c>
+      <c r="K369" t="s">
+        <v>1889</v>
+      </c>
+      <c r="L369">
+        <v>1</v>
+      </c>
+      <c r="M369" t="s">
+        <v>1890</v>
+      </c>
+      <c r="N369">
+        <v>1</v>
+      </c>
+      <c r="O369" t="s">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="370" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A370" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B370" t="s">
+        <v>1893</v>
+      </c>
+      <c r="C370">
+        <v>299.2</v>
+      </c>
+      <c r="D370">
+        <v>201.2</v>
+      </c>
+      <c r="E370">
+        <v>63</v>
+      </c>
+      <c r="F370" t="s">
+        <v>26</v>
+      </c>
+      <c r="G370" t="s">
+        <v>18</v>
+      </c>
+      <c r="H370" t="s">
+        <v>27</v>
+      </c>
+      <c r="I370" t="s">
+        <v>132</v>
+      </c>
+      <c r="J370" t="s">
+        <v>70</v>
+      </c>
+      <c r="K370" t="s">
+        <v>1894</v>
+      </c>
+      <c r="L370">
+        <v>1</v>
+      </c>
+      <c r="M370" t="s">
+        <v>1895</v>
+      </c>
+      <c r="N370">
+        <v>1</v>
+      </c>
+      <c r="O370" t="s">
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="371" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A371" t="s">
+        <v>1897</v>
+      </c>
+      <c r="B371" t="s">
+        <v>1898</v>
+      </c>
+      <c r="C371">
+        <v>311.7</v>
+      </c>
+      <c r="D371">
+        <v>213.6</v>
+      </c>
+      <c r="E371">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="F371" t="s">
+        <v>26</v>
+      </c>
+      <c r="G371" t="s">
+        <v>18</v>
+      </c>
+      <c r="H371" t="s">
+        <v>27</v>
+      </c>
+      <c r="I371" t="s">
+        <v>132</v>
+      </c>
+      <c r="J371" t="s">
+        <v>70</v>
+      </c>
+      <c r="K371" t="s">
+        <v>1899</v>
+      </c>
+      <c r="L371">
+        <v>1</v>
+      </c>
+      <c r="M371" t="s">
+        <v>1900</v>
+      </c>
+      <c r="N371">
+        <v>1</v>
+      </c>
+      <c r="O371" t="s">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="372" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A372" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B372" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C372">
+        <v>18.5</v>
+      </c>
+      <c r="D372">
+        <v>273.5</v>
+      </c>
+      <c r="E372">
+        <v>135.6</v>
+      </c>
+      <c r="F372" t="s">
+        <v>26</v>
+      </c>
+      <c r="G372" t="s">
+        <v>18</v>
+      </c>
+      <c r="H372" t="s">
+        <v>27</v>
+      </c>
+      <c r="I372" t="s">
+        <v>132</v>
+      </c>
+      <c r="J372" t="s">
+        <v>70</v>
+      </c>
+      <c r="K372" t="s">
+        <v>1904</v>
+      </c>
+      <c r="L372">
+        <v>1</v>
+      </c>
+      <c r="M372" t="s">
+        <v>1905</v>
+      </c>
+      <c r="N372">
+        <v>1</v>
+      </c>
+      <c r="O372" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="373" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A373" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B373" t="s">
+        <v>1908</v>
+      </c>
+      <c r="C373">
+        <v>31.4</v>
+      </c>
+      <c r="D373">
+        <v>286.3</v>
+      </c>
+      <c r="E373">
+        <v>148.4</v>
+      </c>
+      <c r="F373" t="s">
+        <v>26</v>
+      </c>
+      <c r="G373" t="s">
+        <v>18</v>
+      </c>
+      <c r="H373" t="s">
+        <v>27</v>
+      </c>
+      <c r="I373" t="s">
+        <v>132</v>
+      </c>
+      <c r="J373" t="s">
+        <v>70</v>
+      </c>
+      <c r="K373" t="s">
+        <v>1909</v>
+      </c>
+      <c r="L373">
+        <v>1</v>
+      </c>
+      <c r="M373" t="s">
+        <v>1910</v>
+      </c>
+      <c r="N373">
+        <v>1</v>
+      </c>
+      <c r="O373" t="s">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="374" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A374" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B374" t="s">
+        <v>1913</v>
+      </c>
+      <c r="C374">
+        <v>44.3</v>
+      </c>
+      <c r="D374">
+        <v>299.10000000000002</v>
+      </c>
+      <c r="E374">
+        <v>161.1</v>
+      </c>
+      <c r="F374" t="s">
+        <v>26</v>
+      </c>
+      <c r="G374" t="s">
+        <v>18</v>
+      </c>
+      <c r="H374" t="s">
+        <v>27</v>
+      </c>
+      <c r="I374" t="s">
+        <v>132</v>
+      </c>
+      <c r="J374" t="s">
+        <v>70</v>
+      </c>
+      <c r="K374" t="s">
+        <v>1914</v>
+      </c>
+      <c r="L374">
+        <v>1</v>
+      </c>
+      <c r="M374" t="s">
+        <v>1915</v>
+      </c>
+      <c r="N374">
+        <v>1</v>
+      </c>
+      <c r="O374" t="s">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="375" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A375" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B375" t="s">
+        <v>1918</v>
+      </c>
+      <c r="C375">
+        <v>57.2</v>
+      </c>
+      <c r="D375">
+        <v>311.89999999999998</v>
+      </c>
+      <c r="E375">
+        <v>173.9</v>
+      </c>
+      <c r="F375" t="s">
+        <v>26</v>
+      </c>
+      <c r="G375" t="s">
+        <v>18</v>
+      </c>
+      <c r="H375" t="s">
+        <v>27</v>
+      </c>
+      <c r="I375" t="s">
+        <v>132</v>
+      </c>
+      <c r="J375" t="s">
+        <v>70</v>
+      </c>
+      <c r="K375" t="s">
+        <v>1919</v>
+      </c>
+      <c r="L375">
+        <v>1</v>
+      </c>
+      <c r="M375" t="s">
+        <v>1920</v>
+      </c>
+      <c r="N375">
+        <v>1</v>
+      </c>
+      <c r="O375" t="s">
+        <v>1921</v>
+      </c>
+    </row>
+    <row r="376" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A376" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B376" t="s">
+        <v>1923</v>
+      </c>
+      <c r="C376">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="D376">
+        <v>324.7</v>
+      </c>
+      <c r="E376">
+        <v>186.8</v>
+      </c>
+      <c r="F376" t="s">
+        <v>26</v>
+      </c>
+      <c r="G376" t="s">
+        <v>18</v>
+      </c>
+      <c r="H376" t="s">
+        <v>27</v>
+      </c>
+      <c r="I376" t="s">
+        <v>132</v>
+      </c>
+      <c r="J376" t="s">
+        <v>70</v>
+      </c>
+      <c r="K376" t="s">
+        <v>1924</v>
+      </c>
+      <c r="L376">
+        <v>1</v>
+      </c>
+      <c r="M376" t="s">
+        <v>1925</v>
+      </c>
+      <c r="N376">
+        <v>1</v>
+      </c>
+      <c r="O376" t="s">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="377" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A377" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B377" t="s">
+        <v>1928</v>
+      </c>
+      <c r="C377">
+        <v>83</v>
+      </c>
+      <c r="D377">
+        <v>337.5</v>
+      </c>
+      <c r="E377">
+        <v>199.5</v>
+      </c>
+      <c r="F377" t="s">
+        <v>26</v>
+      </c>
+      <c r="G377" t="s">
+        <v>18</v>
+      </c>
+      <c r="H377" t="s">
+        <v>27</v>
+      </c>
+      <c r="I377" t="s">
+        <v>132</v>
+      </c>
+      <c r="J377" t="s">
+        <v>70</v>
+      </c>
+      <c r="K377" t="s">
+        <v>1929</v>
+      </c>
+      <c r="L377">
+        <v>1</v>
+      </c>
+      <c r="M377" t="s">
+        <v>1930</v>
+      </c>
+      <c r="N377">
+        <v>1</v>
+      </c>
+      <c r="O377" t="s">
+        <v>1931</v>
+      </c>
+    </row>
+    <row r="378" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A378" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B378" t="s">
+        <v>1933</v>
+      </c>
+      <c r="C378">
+        <v>95.9</v>
+      </c>
+      <c r="D378">
+        <v>350.3</v>
+      </c>
+      <c r="E378">
+        <v>212.3</v>
+      </c>
+      <c r="F378" t="s">
+        <v>26</v>
+      </c>
+      <c r="G378" t="s">
+        <v>18</v>
+      </c>
+      <c r="H378" t="s">
+        <v>27</v>
+      </c>
+      <c r="I378" t="s">
+        <v>132</v>
+      </c>
+      <c r="J378" t="s">
+        <v>70</v>
+      </c>
+      <c r="K378" t="s">
+        <v>1934</v>
+      </c>
+      <c r="L378">
+        <v>1</v>
+      </c>
+      <c r="M378" t="s">
+        <v>1935</v>
+      </c>
+      <c r="N378">
+        <v>1</v>
+      </c>
+      <c r="O378" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="379" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A379" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B379" t="s">
+        <v>1938</v>
+      </c>
+      <c r="C379">
+        <v>108.8</v>
+      </c>
+      <c r="D379">
+        <v>3</v>
+      </c>
+      <c r="E379">
+        <v>225.1</v>
+      </c>
+      <c r="F379" t="s">
+        <v>26</v>
+      </c>
+      <c r="G379" t="s">
+        <v>18</v>
+      </c>
+      <c r="H379" t="s">
+        <v>27</v>
+      </c>
+      <c r="I379" t="s">
+        <v>132</v>
+      </c>
+      <c r="J379" t="s">
+        <v>70</v>
+      </c>
+      <c r="K379" t="s">
+        <v>1939</v>
+      </c>
+      <c r="L379">
+        <v>1</v>
+      </c>
+      <c r="M379" t="s">
+        <v>1940</v>
+      </c>
+      <c r="N379">
+        <v>1</v>
+      </c>
+      <c r="O379" t="s">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="380" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A380" t="s">
+        <v>1942</v>
+      </c>
+      <c r="B380" t="s">
+        <v>1943</v>
+      </c>
+      <c r="C380">
+        <v>258.8</v>
+      </c>
+      <c r="D380">
+        <v>123.6</v>
+      </c>
+      <c r="E380">
+        <v>346.7</v>
+      </c>
+      <c r="F380" t="s">
+        <v>26</v>
+      </c>
+      <c r="G380" t="s">
+        <v>18</v>
+      </c>
+      <c r="H380" t="s">
+        <v>27</v>
+      </c>
+      <c r="I380" t="s">
+        <v>132</v>
+      </c>
+      <c r="J380" t="s">
+        <v>70</v>
+      </c>
+      <c r="K380" t="s">
+        <v>1944</v>
+      </c>
+      <c r="L380">
+        <v>1</v>
+      </c>
+      <c r="M380" t="s">
+        <v>1945</v>
+      </c>
+      <c r="N380">
+        <v>1</v>
+      </c>
+      <c r="O380" t="s">
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="381" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A381" t="s">
+        <v>1947</v>
+      </c>
+      <c r="B381" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C381">
+        <v>271.7</v>
+      </c>
+      <c r="D381">
+        <v>136.30000000000001</v>
+      </c>
+      <c r="E381">
+        <v>359.4</v>
+      </c>
+      <c r="F381" t="s">
+        <v>26</v>
+      </c>
+      <c r="G381" t="s">
+        <v>18</v>
+      </c>
+      <c r="H381" t="s">
+        <v>27</v>
+      </c>
+      <c r="I381" t="s">
+        <v>132</v>
+      </c>
+      <c r="J381" t="s">
+        <v>70</v>
+      </c>
+      <c r="K381" t="s">
+        <v>1949</v>
+      </c>
+      <c r="L381">
+        <v>1</v>
+      </c>
+      <c r="M381" t="s">
+        <v>1950</v>
+      </c>
+      <c r="N381">
+        <v>1</v>
+      </c>
+      <c r="O381" t="s">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="382" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A382" t="s">
+        <v>1952</v>
+      </c>
+      <c r="B382" t="s">
+        <v>1953</v>
+      </c>
+      <c r="C382">
+        <v>284.60000000000002</v>
+      </c>
+      <c r="D382">
+        <v>149.19999999999999</v>
+      </c>
+      <c r="E382">
+        <v>12.2</v>
+      </c>
+      <c r="F382" t="s">
+        <v>26</v>
+      </c>
+      <c r="G382" t="s">
+        <v>18</v>
+      </c>
+      <c r="H382" t="s">
+        <v>27</v>
+      </c>
+      <c r="I382" t="s">
+        <v>132</v>
+      </c>
+      <c r="J382" t="s">
+        <v>70</v>
+      </c>
+      <c r="K382" t="s">
+        <v>1954</v>
+      </c>
+      <c r="L382">
+        <v>1</v>
+      </c>
+      <c r="M382" t="s">
+        <v>1954</v>
+      </c>
+      <c r="N382">
+        <v>1</v>
+      </c>
+      <c r="O382" t="s">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="383" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A383" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B383" t="s">
+        <v>1957</v>
+      </c>
+      <c r="C383">
+        <v>297.5</v>
+      </c>
+      <c r="D383">
+        <v>161.9</v>
+      </c>
+      <c r="E383">
+        <v>25</v>
+      </c>
+      <c r="F383" t="s">
+        <v>26</v>
+      </c>
+      <c r="G383" t="s">
+        <v>18</v>
+      </c>
+      <c r="H383" t="s">
+        <v>27</v>
+      </c>
+      <c r="I383" t="s">
+        <v>132</v>
+      </c>
+      <c r="J383" t="s">
+        <v>70</v>
+      </c>
+      <c r="K383" t="s">
+        <v>1958</v>
+      </c>
+      <c r="L383">
+        <v>1</v>
+      </c>
+      <c r="M383" t="s">
+        <v>1959</v>
+      </c>
+      <c r="N383">
+        <v>1</v>
+      </c>
+      <c r="O383" t="s">
+        <v>1960</v>
+      </c>
+    </row>
+    <row r="384" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A384" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B384" t="s">
+        <v>1962</v>
+      </c>
+      <c r="C384">
+        <v>310.39999999999998</v>
+      </c>
+      <c r="D384">
+        <v>174.7</v>
+      </c>
+      <c r="E384">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="F384" t="s">
+        <v>26</v>
+      </c>
+      <c r="G384" t="s">
+        <v>18</v>
+      </c>
+      <c r="H384" t="s">
+        <v>27</v>
+      </c>
+      <c r="I384" t="s">
+        <v>132</v>
+      </c>
+      <c r="J384" t="s">
+        <v>70</v>
+      </c>
+      <c r="K384" t="s">
+        <v>1963</v>
+      </c>
+      <c r="L384">
+        <v>1</v>
+      </c>
+      <c r="M384" t="s">
+        <v>1964</v>
+      </c>
+      <c r="N384">
+        <v>1</v>
+      </c>
+      <c r="O384" t="s">
+        <v>1965</v>
+      </c>
+    </row>
+    <row r="385" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A385" t="s">
+        <v>1966</v>
+      </c>
+      <c r="B385" t="s">
+        <v>1967</v>
+      </c>
+      <c r="C385">
+        <v>323.3</v>
+      </c>
+      <c r="D385">
+        <v>187.5</v>
+      </c>
+      <c r="E385">
+        <v>50.6</v>
+      </c>
+      <c r="F385" t="s">
+        <v>26</v>
+      </c>
+      <c r="G385" t="s">
+        <v>18</v>
+      </c>
+      <c r="H385" t="s">
+        <v>27</v>
+      </c>
+      <c r="I385" t="s">
+        <v>132</v>
+      </c>
+      <c r="J385" t="s">
+        <v>70</v>
+      </c>
+      <c r="K385" t="s">
+        <v>1968</v>
+      </c>
+      <c r="L385">
+        <v>1</v>
+      </c>
+      <c r="M385" t="s">
+        <v>1969</v>
+      </c>
+      <c r="N385">
+        <v>1</v>
+      </c>
+      <c r="O385" t="s">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="386" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A386" t="s">
+        <v>1971</v>
+      </c>
+      <c r="B386" t="s">
+        <v>1972</v>
+      </c>
+      <c r="C386">
+        <v>336.2</v>
+      </c>
+      <c r="D386">
+        <v>200.3</v>
+      </c>
+      <c r="E386">
+        <v>63.4</v>
+      </c>
+      <c r="F386" t="s">
+        <v>26</v>
+      </c>
+      <c r="G386" t="s">
+        <v>18</v>
+      </c>
+      <c r="H386" t="s">
+        <v>27</v>
+      </c>
+      <c r="I386" t="s">
+        <v>132</v>
+      </c>
+      <c r="J386" t="s">
+        <v>70</v>
+      </c>
+      <c r="K386" t="s">
+        <v>1973</v>
+      </c>
+      <c r="L386">
+        <v>1</v>
+      </c>
+      <c r="M386" t="s">
+        <v>1974</v>
+      </c>
+      <c r="N386">
+        <v>1</v>
+      </c>
+      <c r="O386" t="s">
+        <v>1975</v>
+      </c>
+    </row>
+    <row r="387" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A387" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B387" t="s">
+        <v>1977</v>
+      </c>
+      <c r="C387">
+        <v>349.1</v>
+      </c>
+      <c r="D387">
+        <v>213.1</v>
+      </c>
+      <c r="E387">
+        <v>76.2</v>
+      </c>
+      <c r="F387" t="s">
+        <v>26</v>
+      </c>
+      <c r="G387" t="s">
+        <v>18</v>
+      </c>
+      <c r="H387" t="s">
+        <v>27</v>
+      </c>
+      <c r="I387" t="s">
+        <v>132</v>
+      </c>
+      <c r="J387" t="s">
+        <v>70</v>
+      </c>
+      <c r="K387" t="s">
+        <v>1978</v>
+      </c>
+      <c r="L387">
+        <v>1</v>
+      </c>
+      <c r="M387" t="s">
+        <v>1979</v>
+      </c>
+      <c r="N387">
+        <v>1</v>
+      </c>
+      <c r="O387" t="s">
+        <v>1980</v>
+      </c>
+    </row>
+    <row r="388" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A388" t="s">
+        <v>1981</v>
+      </c>
+      <c r="B388" t="s">
+        <v>1982</v>
+      </c>
+      <c r="C388">
+        <v>2</v>
+      </c>
+      <c r="D388">
+        <v>225.8</v>
+      </c>
+      <c r="E388">
+        <v>89</v>
+      </c>
+      <c r="F388" t="s">
+        <v>26</v>
+      </c>
+      <c r="G388" t="s">
+        <v>18</v>
+      </c>
+      <c r="H388" t="s">
+        <v>27</v>
+      </c>
+      <c r="I388" t="s">
+        <v>132</v>
+      </c>
+      <c r="J388" t="s">
+        <v>70</v>
+      </c>
+      <c r="K388" t="s">
+        <v>1983</v>
+      </c>
+      <c r="L388">
+        <v>1</v>
+      </c>
+      <c r="M388" t="s">
+        <v>1984</v>
+      </c>
+      <c r="N388">
+        <v>1</v>
+      </c>
+      <c r="O388" t="s">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="389" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A389" t="s">
+        <v>1986</v>
+      </c>
+      <c r="B389" t="s">
+        <v>1987</v>
+      </c>
+      <c r="C389">
+        <v>14.9</v>
+      </c>
+      <c r="D389">
+        <v>238.7</v>
+      </c>
+      <c r="E389">
+        <v>101.8</v>
+      </c>
+      <c r="F389" t="s">
+        <v>26</v>
+      </c>
+      <c r="G389" t="s">
+        <v>18</v>
+      </c>
+      <c r="H389" t="s">
+        <v>27</v>
+      </c>
+      <c r="I389" t="s">
+        <v>132</v>
+      </c>
+      <c r="J389" t="s">
+        <v>70</v>
+      </c>
+      <c r="K389" t="s">
+        <v>1988</v>
+      </c>
+      <c r="L389">
+        <v>1</v>
+      </c>
+      <c r="M389" t="s">
+        <v>1989</v>
+      </c>
+      <c r="N389">
+        <v>1</v>
+      </c>
+      <c r="O389" t="s">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="390" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A390" t="s">
+        <v>1991</v>
+      </c>
+      <c r="B390" t="s">
+        <v>1992</v>
+      </c>
+      <c r="C390">
+        <v>57.1</v>
+      </c>
+      <c r="D390">
+        <v>274.2</v>
+      </c>
+      <c r="E390">
+        <v>137.6</v>
+      </c>
+      <c r="F390" t="s">
+        <v>26</v>
+      </c>
+      <c r="G390" t="s">
+        <v>18</v>
+      </c>
+      <c r="H390" t="s">
+        <v>27</v>
+      </c>
+      <c r="I390" t="s">
+        <v>132</v>
+      </c>
+      <c r="J390" t="s">
+        <v>70</v>
+      </c>
+      <c r="K390" t="s">
+        <v>1993</v>
+      </c>
+      <c r="L390">
+        <v>1</v>
+      </c>
+      <c r="M390" t="s">
+        <v>1994</v>
+      </c>
+      <c r="N390">
+        <v>1</v>
+      </c>
+      <c r="O390" t="s">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="391" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A391" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B391" t="s">
+        <v>1997</v>
+      </c>
+      <c r="C391">
+        <v>70</v>
+      </c>
+      <c r="D391">
+        <v>287.10000000000002</v>
+      </c>
+      <c r="E391">
+        <v>150.4</v>
+      </c>
+      <c r="F391" t="s">
+        <v>26</v>
+      </c>
+      <c r="G391" t="s">
+        <v>18</v>
+      </c>
+      <c r="H391" t="s">
+        <v>27</v>
+      </c>
+      <c r="I391" t="s">
+        <v>132</v>
+      </c>
+      <c r="J391" t="s">
+        <v>70</v>
+      </c>
+      <c r="K391" t="s">
+        <v>1998</v>
+      </c>
+      <c r="L391">
+        <v>1</v>
+      </c>
+      <c r="M391" t="s">
+        <v>1999</v>
+      </c>
+      <c r="N391">
+        <v>1</v>
+      </c>
+      <c r="O391" t="s">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="392" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A392" t="s">
+        <v>2001</v>
+      </c>
+      <c r="B392" t="s">
+        <v>2002</v>
+      </c>
+      <c r="C392">
+        <v>82.9</v>
+      </c>
+      <c r="D392">
+        <v>299.89999999999998</v>
+      </c>
+      <c r="E392">
+        <v>163.19999999999999</v>
+      </c>
+      <c r="F392" t="s">
+        <v>26</v>
+      </c>
+      <c r="G392" t="s">
+        <v>18</v>
+      </c>
+      <c r="H392" t="s">
+        <v>27</v>
+      </c>
+      <c r="I392" t="s">
+        <v>132</v>
+      </c>
+      <c r="J392" t="s">
+        <v>70</v>
+      </c>
+      <c r="K392" t="s">
+        <v>2003</v>
+      </c>
+      <c r="L392">
+        <v>1</v>
+      </c>
+      <c r="M392" t="s">
+        <v>2004</v>
+      </c>
+      <c r="N392">
+        <v>1</v>
+      </c>
+      <c r="O392" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="393" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A393" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B393" t="s">
+        <v>2007</v>
+      </c>
+      <c r="C393">
+        <v>95.8</v>
+      </c>
+      <c r="D393">
+        <v>312.60000000000002</v>
+      </c>
+      <c r="E393">
+        <v>176</v>
+      </c>
+      <c r="F393" t="s">
+        <v>26</v>
+      </c>
+      <c r="G393" t="s">
+        <v>18</v>
+      </c>
+      <c r="H393" t="s">
+        <v>27</v>
+      </c>
+      <c r="I393" t="s">
+        <v>132</v>
+      </c>
+      <c r="J393" t="s">
+        <v>70</v>
+      </c>
+      <c r="K393" t="s">
+        <v>2008</v>
+      </c>
+      <c r="L393">
+        <v>1</v>
+      </c>
+      <c r="M393" t="s">
+        <v>2009</v>
+      </c>
+      <c r="N393">
+        <v>1</v>
+      </c>
+      <c r="O393" t="s">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="394" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A394" t="s">
+        <v>2011</v>
+      </c>
+      <c r="B394" t="s">
+        <v>2012</v>
+      </c>
+      <c r="C394">
+        <v>108.6</v>
+      </c>
+      <c r="D394">
+        <v>325.2</v>
+      </c>
+      <c r="E394">
+        <v>188.6</v>
+      </c>
+      <c r="F394" t="s">
+        <v>26</v>
+      </c>
+      <c r="G394" t="s">
+        <v>18</v>
+      </c>
+      <c r="H394" t="s">
+        <v>27</v>
+      </c>
+      <c r="I394" t="s">
+        <v>132</v>
+      </c>
+      <c r="J394" t="s">
+        <v>70</v>
+      </c>
+      <c r="K394" t="s">
+        <v>2013</v>
+      </c>
+      <c r="L394">
+        <v>1</v>
+      </c>
+      <c r="M394" t="s">
+        <v>2014</v>
+      </c>
+      <c r="N394">
+        <v>1</v>
+      </c>
+      <c r="O394" t="s">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="395" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A395" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B395" t="s">
+        <v>2017</v>
+      </c>
+      <c r="C395">
+        <v>121.6</v>
+      </c>
+      <c r="D395">
+        <v>338.2</v>
+      </c>
+      <c r="E395">
+        <v>201.5</v>
+      </c>
+      <c r="F395" t="s">
+        <v>26</v>
+      </c>
+      <c r="G395" t="s">
+        <v>18</v>
+      </c>
+      <c r="H395" t="s">
+        <v>27</v>
+      </c>
+      <c r="I395" t="s">
+        <v>132</v>
+      </c>
+      <c r="J395" t="s">
+        <v>70</v>
+      </c>
+      <c r="K395" t="s">
+        <v>2018</v>
+      </c>
+      <c r="L395">
+        <v>1</v>
+      </c>
+      <c r="M395" t="s">
+        <v>2019</v>
+      </c>
+      <c r="N395">
+        <v>1</v>
+      </c>
+      <c r="O395" t="s">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="396" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A396" t="s">
+        <v>2021</v>
+      </c>
+      <c r="B396" t="s">
+        <v>2022</v>
+      </c>
+      <c r="C396">
+        <v>134.5</v>
+      </c>
+      <c r="D396">
+        <v>351</v>
+      </c>
+      <c r="E396">
+        <v>214.4</v>
+      </c>
+      <c r="F396" t="s">
+        <v>26</v>
+      </c>
+      <c r="G396" t="s">
+        <v>18</v>
+      </c>
+      <c r="H396" t="s">
+        <v>27</v>
+      </c>
+      <c r="I396" t="s">
+        <v>132</v>
+      </c>
+      <c r="J396" t="s">
+        <v>70</v>
+      </c>
+      <c r="K396" t="s">
+        <v>2023</v>
+      </c>
+      <c r="L396">
+        <v>1</v>
+      </c>
+      <c r="M396" t="s">
+        <v>2024</v>
+      </c>
+      <c r="N396">
+        <v>1</v>
+      </c>
+      <c r="O396" t="s">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="397" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A397" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B397" t="s">
+        <v>2027</v>
+      </c>
+      <c r="C397">
+        <v>147.4</v>
+      </c>
+      <c r="D397">
+        <v>3.7</v>
+      </c>
+      <c r="E397">
+        <v>227.1</v>
+      </c>
+      <c r="F397" t="s">
+        <v>26</v>
+      </c>
+      <c r="G397" t="s">
+        <v>18</v>
+      </c>
+      <c r="H397" t="s">
+        <v>27</v>
+      </c>
+      <c r="I397" t="s">
+        <v>132</v>
+      </c>
+      <c r="J397" t="s">
+        <v>70</v>
+      </c>
+      <c r="K397" t="s">
+        <v>2028</v>
+      </c>
+      <c r="L397">
+        <v>1</v>
+      </c>
+      <c r="M397" t="s">
+        <v>2029</v>
+      </c>
+      <c r="N397">
+        <v>1</v>
+      </c>
+      <c r="O397" t="s">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="398" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A398" t="s">
+        <v>2031</v>
+      </c>
+      <c r="B398" t="s">
+        <v>2032</v>
+      </c>
+      <c r="C398">
+        <v>160.30000000000001</v>
+      </c>
+      <c r="D398">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E398">
+        <v>239.9</v>
+      </c>
+      <c r="F398" t="s">
+        <v>26</v>
+      </c>
+      <c r="G398" t="s">
+        <v>18</v>
+      </c>
+      <c r="H398" t="s">
+        <v>27</v>
+      </c>
+      <c r="I398" t="s">
+        <v>132</v>
+      </c>
+      <c r="J398" t="s">
+        <v>70</v>
+      </c>
+      <c r="K398" t="s">
+        <v>2033</v>
+      </c>
+      <c r="L398">
+        <v>1</v>
+      </c>
+      <c r="M398" t="s">
+        <v>2034</v>
+      </c>
+      <c r="N398">
+        <v>1</v>
+      </c>
+      <c r="O398" t="s">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="399" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A399" t="s">
+        <v>2036</v>
+      </c>
+      <c r="B399" t="s">
+        <v>2037</v>
+      </c>
+      <c r="C399">
+        <v>173.2</v>
+      </c>
+      <c r="D399">
+        <v>29.4</v>
+      </c>
+      <c r="E399">
+        <v>252.7</v>
+      </c>
+      <c r="F399" t="s">
+        <v>26</v>
+      </c>
+      <c r="G399" t="s">
+        <v>18</v>
+      </c>
+      <c r="H399" t="s">
+        <v>27</v>
+      </c>
+      <c r="I399" t="s">
+        <v>132</v>
+      </c>
+      <c r="J399" t="s">
+        <v>70</v>
+      </c>
+      <c r="K399" t="s">
+        <v>2038</v>
+      </c>
+      <c r="L399">
+        <v>1</v>
+      </c>
+      <c r="M399" t="s">
+        <v>2039</v>
+      </c>
+      <c r="N399">
+        <v>1</v>
+      </c>
+      <c r="O399" t="s">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="400" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A400" t="s">
+        <v>2041</v>
+      </c>
+      <c r="B400" t="s">
+        <v>2042</v>
+      </c>
+      <c r="C400">
+        <v>186.1</v>
+      </c>
+      <c r="D400">
+        <v>42.1</v>
+      </c>
+      <c r="E400">
+        <v>265.5</v>
+      </c>
+      <c r="F400" t="s">
+        <v>26</v>
+      </c>
+      <c r="G400" t="s">
+        <v>18</v>
+      </c>
+      <c r="H400" t="s">
+        <v>27</v>
+      </c>
+      <c r="I400" t="s">
+        <v>132</v>
+      </c>
+      <c r="J400" t="s">
+        <v>70</v>
+      </c>
+      <c r="K400" t="s">
+        <v>2043</v>
+      </c>
+      <c r="L400">
+        <v>1</v>
+      </c>
+      <c r="M400" t="s">
+        <v>2044</v>
+      </c>
+      <c r="N400">
+        <v>1</v>
+      </c>
+      <c r="O400" t="s">
+        <v>2040</v>
       </c>
     </row>
   </sheetData>
@@ -26084,11 +28753,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FB822E-4FB0-4362-8846-871BD8F7A1EF}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26104,8 +28773,8 @@
         <v>685</v>
       </c>
       <c r="B1" s="18">
-        <f>SUM(B2:B99)</f>
-        <v>421</v>
+        <f>SUM(B2:B100)</f>
+        <v>532</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>696</v>
@@ -26823,8 +29492,11 @@
       <c r="B47">
         <v>9</v>
       </c>
+      <c r="C47" t="s">
+        <v>687</v>
+      </c>
       <c r="D47" t="s">
-        <v>910</v>
+        <v>695</v>
       </c>
       <c r="E47" t="s">
         <v>1831</v>
@@ -26837,8 +29509,111 @@
       <c r="B48">
         <v>9</v>
       </c>
+      <c r="C48" t="s">
+        <v>687</v>
+      </c>
+      <c r="D48" t="s">
+        <v>695</v>
+      </c>
       <c r="E48" t="s">
         <v>1831</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="32">
+        <v>45939</v>
+      </c>
+      <c r="B49">
+        <v>11</v>
+      </c>
+      <c r="C49" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="32">
+        <v>45942</v>
+      </c>
+      <c r="B50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="32">
+        <v>45946</v>
+      </c>
+      <c r="B51">
+        <v>14</v>
+      </c>
+      <c r="C51" t="s">
+        <v>687</v>
+      </c>
+      <c r="D51" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="32">
+        <v>45947</v>
+      </c>
+      <c r="B52">
+        <v>12</v>
+      </c>
+      <c r="C52" t="s">
+        <v>687</v>
+      </c>
+      <c r="D52" t="s">
+        <v>695</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="32">
+        <v>45949</v>
+      </c>
+      <c r="B53">
+        <v>15</v>
+      </c>
+      <c r="C53" t="s">
+        <v>687</v>
+      </c>
+      <c r="D53" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="32">
+        <v>45950</v>
+      </c>
+      <c r="B54">
+        <v>16</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="32">
+        <v>45959</v>
+      </c>
+      <c r="B55">
+        <v>18</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="32">
+        <v>45960</v>
+      </c>
+      <c r="B56">
+        <v>10</v>
+      </c>
+      <c r="E56" t="s">
+        <v>2047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearchitected parts of NEZ features and outside data sources
Changes locations and organization of HST data and made NEZ feature codes work with that. Next up is to reorganize other outside data like 889nm and 5-micron data
</commit_message>
<xml_diff>
--- a/Catalog/Catalog-static.xlsx
+++ b/Catalog/Catalog-static.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Astronomy\Projects\SAS 2021 Ammonia\Jupiter_NH3_Analysis_P3\Catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD0EF73-A6A2-48B7-ABAD-847C45E95D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A7DC70-4E54-446D-A224-0DF26005EE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalog-static" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5869" uniqueCount="2446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5874" uniqueCount="2451">
   <si>
     <t>ObsID</t>
   </si>
@@ -7481,6 +7481,21 @@
   </si>
   <si>
     <t>Very clear, fair seeing</t>
+  </si>
+  <si>
+    <t>Very clear. Good seeing once Jupiter was high enough above the horizon</t>
+  </si>
+  <si>
+    <t>Very clear, very good seeing (expected from GFS). Extraordinary seeing at 11:35pm LT</t>
+  </si>
+  <si>
+    <t>Very clear, very good seeing (not quite as good as the prior night)</t>
+  </si>
+  <si>
+    <t>Very clear, good seeing</t>
+  </si>
+  <si>
+    <t>Very clear, very good seeing. Had power interrupt lost 20 mins, then later found mount clock was wrong and lost about 65 mins around flip</t>
   </si>
 </sst>
 </file>
@@ -7670,7 +7685,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="47">
+  <fills count="48">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7934,6 +7949,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -8095,7 +8116,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -8196,6 +8217,7 @@
     <xf numFmtId="165" fontId="16" fillId="46" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -40315,7 +40337,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40332,7 +40354,7 @@
       </c>
       <c r="B1" s="18">
         <f>SUM(B2:B101)</f>
-        <v>853</v>
+        <v>986</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>696</v>
@@ -41103,7 +41125,7 @@
       <c r="C51" t="s">
         <v>687</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="51" t="s">
         <v>695</v>
       </c>
     </row>
@@ -41117,7 +41139,7 @@
       <c r="C52" t="s">
         <v>687</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="51" t="s">
         <v>695</v>
       </c>
       <c r="E52" t="s">
@@ -41134,7 +41156,7 @@
       <c r="C53" t="s">
         <v>687</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="51" t="s">
         <v>695</v>
       </c>
     </row>
@@ -41145,7 +41167,7 @@
       <c r="B54">
         <v>16</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="51" t="s">
         <v>695</v>
       </c>
       <c r="E54" t="s">
@@ -41258,7 +41280,7 @@
       <c r="B64">
         <v>21</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="51" t="s">
         <v>695</v>
       </c>
       <c r="E64" s="18" t="s">
@@ -41272,7 +41294,7 @@
       <c r="B65">
         <v>20</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="51" t="s">
         <v>695</v>
       </c>
       <c r="E65" t="s">
@@ -41375,6 +41397,7 @@
         <f>198/22</f>
         <v>9</v>
       </c>
+      <c r="D74" s="51"/>
       <c r="E74" s="18" t="s">
         <v>2438</v>
       </c>
@@ -41386,6 +41409,7 @@
       <c r="B75">
         <v>27</v>
       </c>
+      <c r="D75" s="51"/>
       <c r="E75" t="s">
         <v>2439</v>
       </c>
@@ -41397,40 +41421,85 @@
       <c r="B76">
         <v>19</v>
       </c>
+      <c r="D76" s="58"/>
       <c r="E76" t="s">
         <v>2440</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
-        <v>46012</v>
+        <v>46013</v>
       </c>
       <c r="B77">
         <v>28</v>
       </c>
+      <c r="D77" s="58"/>
       <c r="E77" t="s">
         <v>2445</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" s="30"/>
+      <c r="A78" s="30">
+        <v>46017</v>
+      </c>
+      <c r="B78">
+        <v>26</v>
+      </c>
+      <c r="D78" s="51"/>
+      <c r="E78" t="s">
+        <v>2446</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="30"/>
+      <c r="A79" s="30">
+        <v>46021</v>
+      </c>
+      <c r="B79">
+        <v>27</v>
+      </c>
+      <c r="D79" s="51"/>
+      <c r="E79" t="s">
+        <v>2447</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="30"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="30"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="30"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="30">
+        <v>46022</v>
+      </c>
+      <c r="B80">
+        <v>28</v>
+      </c>
+      <c r="D80" s="51"/>
+      <c r="E80" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="30">
+        <v>46028</v>
+      </c>
+      <c r="B81">
+        <v>26</v>
+      </c>
+      <c r="E81" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" s="30">
+        <v>46033</v>
+      </c>
+      <c r="B82">
+        <v>26</v>
+      </c>
+      <c r="E82" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="30"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="30"/>
       <c r="B84" s="30"/>
     </row>

</xml_diff>